<commit_message>
Adding Homs Ammo factory, updating progress.
</commit_message>
<xml_diff>
--- a/UNDER DEVELOPMENT/OPAR Version 2/JESTER/OPAR v2.0_JOINT_TARGET_LIST_JESTER.xlsx
+++ b/UNDER DEVELOPMENT/OPAR Version 2/JESTER/OPAR v2.0_JOINT_TARGET_LIST_JESTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\132nd\02 Operations\OPAR\V2\OPAR_BRIEF\UNDER DEVELOPMENT\OPAR Version 2\JESTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0817544C-9783-447F-9F0A-5B9913721115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA74F360-EA13-4701-8F25-0BAB21A7AFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6203,9 +6203,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A18" sqref="A18:B18"/>
+      <selection pane="topRight" activeCell="B19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6636,11 +6636,11 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="160" t="s">
+      <c r="A19" s="238" t="s">
         <v>97</v>
       </c>
-      <c r="B19" s="156" t="s">
-        <v>98</v>
+      <c r="B19" s="240" t="s">
+        <v>65</v>
       </c>
       <c r="C19" s="204" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Adding Opartgt027 ( god help us all) and updating progress.
</commit_message>
<xml_diff>
--- a/UNDER DEVELOPMENT/OPAR Version 2/JESTER/OPAR v2.0_JOINT_TARGET_LIST_JESTER.xlsx
+++ b/UNDER DEVELOPMENT/OPAR Version 2/JESTER/OPAR v2.0_JOINT_TARGET_LIST_JESTER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\132nd\02 Operations\OPAR\V2\OPAR_BRIEF\UNDER DEVELOPMENT\OPAR Version 2\JESTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FADE80D-F95D-4E26-8B54-6E9B0D70611F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2925550B-F88E-442D-9B18-F523F9310632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17040" yWindow="5120" windowWidth="17340" windowHeight="15030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Target List" sheetId="1" r:id="rId1"/>
@@ -4301,26 +4301,21 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="10" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4332,16 +4327,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4350,9 +4353,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -6203,9 +6203,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A20" sqref="A20:B20"/>
+      <selection pane="topRight" activeCell="A29" sqref="A29:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6851,10 +6851,10 @@
       <c r="I26" s="222"/>
     </row>
     <row r="27" spans="1:26" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="160" t="s">
+      <c r="A27" s="238" t="s">
         <v>147</v>
       </c>
-      <c r="B27" s="156" t="s">
+      <c r="B27" s="240" t="s">
         <v>148</v>
       </c>
       <c r="C27" s="204" t="s">
@@ -6876,10 +6876,10 @@
       <c r="I27" s="222"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="158" t="s">
+      <c r="A28" s="237" t="s">
         <v>153</v>
       </c>
-      <c r="B28" s="152" t="s">
+      <c r="B28" s="239" t="s">
         <v>154</v>
       </c>
       <c r="C28" s="200" t="s">
@@ -6901,10 +6901,10 @@
       <c r="I28" s="222"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="160" t="s">
+      <c r="A29" s="238" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="156" t="s">
+      <c r="B29" s="240" t="s">
         <v>160</v>
       </c>
       <c r="C29" s="204" t="s">
@@ -6926,10 +6926,10 @@
       <c r="I29" s="223"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="158" t="s">
+      <c r="A30" s="237" t="s">
         <v>166</v>
       </c>
-      <c r="B30" s="152" t="s">
+      <c r="B30" s="239" t="s">
         <v>167</v>
       </c>
       <c r="C30" s="200" t="s">
@@ -15799,33 +15799,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="244" t="s">
+      <c r="A1" s="260" t="s">
         <v>630</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="246"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="262"/>
     </row>
     <row r="2" spans="1:11" ht="14" x14ac:dyDescent="0.3">
-      <c r="A2" s="247" t="s">
+      <c r="A2" s="263" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="248"/>
       <c r="C2" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="249" t="s">
+      <c r="D2" s="264" t="s">
         <v>632</v>
       </c>
-      <c r="E2" s="250"/>
-      <c r="F2" s="250"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
       <c r="G2" s="248"/>
-      <c r="H2" s="251"/>
+      <c r="H2" s="265"/>
       <c r="I2" s="252"/>
     </row>
     <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -15834,17 +15834,17 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="253" t="s">
+      <c r="A4" s="266" t="s">
         <v>634</v>
       </c>
-      <c r="B4" s="245"/>
-      <c r="C4" s="245"/>
-      <c r="D4" s="245"/>
-      <c r="E4" s="245"/>
-      <c r="F4" s="245"/>
-      <c r="G4" s="245"/>
-      <c r="H4" s="245"/>
-      <c r="I4" s="246"/>
+      <c r="B4" s="261"/>
+      <c r="C4" s="261"/>
+      <c r="D4" s="261"/>
+      <c r="E4" s="261"/>
+      <c r="F4" s="261"/>
+      <c r="G4" s="261"/>
+      <c r="H4" s="261"/>
+      <c r="I4" s="262"/>
     </row>
     <row r="5" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="85" t="s">
@@ -15991,17 +15991,17 @@
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="254" t="s">
+      <c r="A15" s="253" t="s">
         <v>641</v>
       </c>
-      <c r="B15" s="255"/>
-      <c r="C15" s="255"/>
-      <c r="D15" s="255"/>
-      <c r="E15" s="255"/>
-      <c r="F15" s="255"/>
-      <c r="G15" s="255"/>
-      <c r="H15" s="255"/>
-      <c r="I15" s="256"/>
+      <c r="B15" s="254"/>
+      <c r="C15" s="254"/>
+      <c r="D15" s="254"/>
+      <c r="E15" s="254"/>
+      <c r="F15" s="254"/>
+      <c r="G15" s="254"/>
+      <c r="H15" s="254"/>
+      <c r="I15" s="255"/>
     </row>
     <row r="16" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" s="89" t="s">
@@ -16016,15 +16016,15 @@
       <c r="D16" s="90" t="s">
         <v>640</v>
       </c>
-      <c r="E16" s="257" t="s">
+      <c r="E16" s="256" t="s">
         <v>642</v>
       </c>
-      <c r="F16" s="260"/>
-      <c r="G16" s="257" t="s">
+      <c r="F16" s="259"/>
+      <c r="G16" s="256" t="s">
         <v>643</v>
       </c>
-      <c r="H16" s="258"/>
-      <c r="I16" s="259"/>
+      <c r="H16" s="257"/>
+      <c r="I16" s="258"/>
     </row>
     <row r="17" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="91">
@@ -16033,11 +16033,11 @@
       <c r="B17" s="92"/>
       <c r="C17" s="92"/>
       <c r="D17" s="92"/>
-      <c r="E17" s="261"/>
-      <c r="F17" s="262"/>
-      <c r="G17" s="261"/>
-      <c r="H17" s="263"/>
-      <c r="I17" s="264"/>
+      <c r="E17" s="244"/>
+      <c r="F17" s="245"/>
+      <c r="G17" s="244"/>
+      <c r="H17" s="249"/>
+      <c r="I17" s="250"/>
       <c r="K17" s="84" t="s">
         <v>646</v>
       </c>
@@ -16049,11 +16049,11 @@
       <c r="B18" s="92"/>
       <c r="C18" s="92"/>
       <c r="D18" s="92"/>
-      <c r="E18" s="261"/>
-      <c r="F18" s="262"/>
-      <c r="G18" s="261"/>
-      <c r="H18" s="263"/>
-      <c r="I18" s="264"/>
+      <c r="E18" s="244"/>
+      <c r="F18" s="245"/>
+      <c r="G18" s="244"/>
+      <c r="H18" s="249"/>
+      <c r="I18" s="250"/>
     </row>
     <row r="19" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="91">
@@ -16062,11 +16062,11 @@
       <c r="B19" s="92"/>
       <c r="C19" s="92"/>
       <c r="D19" s="92"/>
-      <c r="E19" s="261"/>
-      <c r="F19" s="262"/>
-      <c r="G19" s="261"/>
-      <c r="H19" s="263"/>
-      <c r="I19" s="264"/>
+      <c r="E19" s="244"/>
+      <c r="F19" s="245"/>
+      <c r="G19" s="244"/>
+      <c r="H19" s="249"/>
+      <c r="I19" s="250"/>
     </row>
     <row r="20" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="91">
@@ -16075,11 +16075,11 @@
       <c r="B20" s="92"/>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
-      <c r="E20" s="261"/>
-      <c r="F20" s="262"/>
-      <c r="G20" s="261"/>
-      <c r="H20" s="263"/>
-      <c r="I20" s="264"/>
+      <c r="E20" s="244"/>
+      <c r="F20" s="245"/>
+      <c r="G20" s="244"/>
+      <c r="H20" s="249"/>
+      <c r="I20" s="250"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="91">
@@ -16088,11 +16088,11 @@
       <c r="B21" s="92"/>
       <c r="C21" s="92"/>
       <c r="D21" s="92"/>
-      <c r="E21" s="261"/>
-      <c r="F21" s="262"/>
-      <c r="G21" s="261"/>
-      <c r="H21" s="263"/>
-      <c r="I21" s="264"/>
+      <c r="E21" s="244"/>
+      <c r="F21" s="245"/>
+      <c r="G21" s="244"/>
+      <c r="H21" s="249"/>
+      <c r="I21" s="250"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="91">
@@ -16101,11 +16101,11 @@
       <c r="B22" s="92"/>
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
-      <c r="E22" s="261"/>
-      <c r="F22" s="262"/>
-      <c r="G22" s="261"/>
-      <c r="H22" s="263"/>
-      <c r="I22" s="264"/>
+      <c r="E22" s="244"/>
+      <c r="F22" s="245"/>
+      <c r="G22" s="244"/>
+      <c r="H22" s="249"/>
+      <c r="I22" s="250"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="91">
@@ -16114,11 +16114,11 @@
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
       <c r="D23" s="92"/>
-      <c r="E23" s="261"/>
-      <c r="F23" s="262"/>
-      <c r="G23" s="261"/>
-      <c r="H23" s="263"/>
-      <c r="I23" s="264"/>
+      <c r="E23" s="244"/>
+      <c r="F23" s="245"/>
+      <c r="G23" s="244"/>
+      <c r="H23" s="249"/>
+      <c r="I23" s="250"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="91">
@@ -16127,11 +16127,11 @@
       <c r="B24" s="92"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
-      <c r="E24" s="261"/>
-      <c r="F24" s="262"/>
-      <c r="G24" s="261"/>
-      <c r="H24" s="263"/>
-      <c r="I24" s="264"/>
+      <c r="E24" s="244"/>
+      <c r="F24" s="245"/>
+      <c r="G24" s="244"/>
+      <c r="H24" s="249"/>
+      <c r="I24" s="250"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="91">
@@ -16140,11 +16140,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="265"/>
-      <c r="F25" s="262"/>
-      <c r="G25" s="265"/>
-      <c r="H25" s="263"/>
-      <c r="I25" s="264"/>
+      <c r="E25" s="246"/>
+      <c r="F25" s="245"/>
+      <c r="G25" s="246"/>
+      <c r="H25" s="249"/>
+      <c r="I25" s="250"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="94">
@@ -16153,10 +16153,10 @@
       <c r="B26" s="95"/>
       <c r="C26" s="95"/>
       <c r="D26" s="95"/>
-      <c r="E26" s="266"/>
+      <c r="E26" s="247"/>
       <c r="F26" s="248"/>
-      <c r="G26" s="266"/>
-      <c r="H26" s="250"/>
+      <c r="G26" s="247"/>
+      <c r="H26" s="251"/>
       <c r="I26" s="252"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17135,12 +17135,16 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:I18"/>
     <mergeCell ref="E19:F19"/>
@@ -17153,16 +17157,12 @@
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="G22:I22"/>
     <mergeCell ref="G23:I23"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -17193,49 +17193,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="244" t="s">
+      <c r="A1" s="260" t="s">
         <v>630</v>
       </c>
-      <c r="B1" s="245"/>
-      <c r="C1" s="245"/>
-      <c r="D1" s="245"/>
-      <c r="E1" s="245"/>
-      <c r="F1" s="245"/>
-      <c r="G1" s="245"/>
-      <c r="H1" s="245"/>
-      <c r="I1" s="246"/>
+      <c r="B1" s="261"/>
+      <c r="C1" s="261"/>
+      <c r="D1" s="261"/>
+      <c r="E1" s="261"/>
+      <c r="F1" s="261"/>
+      <c r="G1" s="261"/>
+      <c r="H1" s="261"/>
+      <c r="I1" s="262"/>
     </row>
     <row r="2" spans="1:17" ht="14" x14ac:dyDescent="0.3">
-      <c r="A2" s="247" t="s">
+      <c r="A2" s="263" t="s">
         <v>631</v>
       </c>
       <c r="B2" s="248"/>
       <c r="C2" s="100" t="s">
         <v>655</v>
       </c>
-      <c r="D2" s="249" t="s">
+      <c r="D2" s="264" t="s">
         <v>632</v>
       </c>
-      <c r="E2" s="250"/>
-      <c r="F2" s="250"/>
+      <c r="E2" s="251"/>
+      <c r="F2" s="251"/>
       <c r="G2" s="248"/>
-      <c r="H2" s="251" t="s">
+      <c r="H2" s="265" t="s">
         <v>656</v>
       </c>
       <c r="I2" s="252"/>
     </row>
     <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="253" t="s">
+      <c r="A4" s="266" t="s">
         <v>634</v>
       </c>
-      <c r="B4" s="245"/>
-      <c r="C4" s="245"/>
-      <c r="D4" s="245"/>
-      <c r="E4" s="245"/>
-      <c r="F4" s="245"/>
-      <c r="G4" s="245"/>
-      <c r="H4" s="245"/>
-      <c r="I4" s="246"/>
+      <c r="B4" s="261"/>
+      <c r="C4" s="261"/>
+      <c r="D4" s="261"/>
+      <c r="E4" s="261"/>
+      <c r="F4" s="261"/>
+      <c r="G4" s="261"/>
+      <c r="H4" s="261"/>
+      <c r="I4" s="262"/>
     </row>
     <row r="5" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="85" t="s">
@@ -17297,15 +17297,15 @@
       <c r="I6" s="97" t="s">
         <v>664</v>
       </c>
-      <c r="K6" s="267" t="s">
+      <c r="K6" s="268" t="s">
         <v>665</v>
       </c>
-      <c r="L6" s="268"/>
-      <c r="M6" s="268"/>
-      <c r="N6" s="268"/>
-      <c r="O6" s="268"/>
-      <c r="P6" s="268"/>
-      <c r="Q6" s="268"/>
+      <c r="L6" s="269"/>
+      <c r="M6" s="269"/>
+      <c r="N6" s="269"/>
+      <c r="O6" s="269"/>
+      <c r="P6" s="269"/>
+      <c r="Q6" s="269"/>
     </row>
     <row r="7" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="96">
@@ -17335,15 +17335,15 @@
       <c r="I7" s="97" t="s">
         <v>672</v>
       </c>
-      <c r="K7" s="267" t="s">
+      <c r="K7" s="268" t="s">
         <v>673</v>
       </c>
-      <c r="L7" s="268"/>
-      <c r="M7" s="268"/>
-      <c r="N7" s="268"/>
-      <c r="O7" s="268"/>
-      <c r="P7" s="268"/>
-      <c r="Q7" s="268"/>
+      <c r="L7" s="269"/>
+      <c r="M7" s="269"/>
+      <c r="N7" s="269"/>
+      <c r="O7" s="269"/>
+      <c r="P7" s="269"/>
+      <c r="Q7" s="269"/>
     </row>
     <row r="8" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="96">
@@ -17451,17 +17451,17 @@
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="254" t="s">
+      <c r="A15" s="253" t="s">
         <v>641</v>
       </c>
-      <c r="B15" s="255"/>
-      <c r="C15" s="255"/>
-      <c r="D15" s="255"/>
-      <c r="E15" s="255"/>
-      <c r="F15" s="255"/>
-      <c r="G15" s="255"/>
-      <c r="H15" s="255"/>
-      <c r="I15" s="256"/>
+      <c r="B15" s="254"/>
+      <c r="C15" s="254"/>
+      <c r="D15" s="254"/>
+      <c r="E15" s="254"/>
+      <c r="F15" s="254"/>
+      <c r="G15" s="254"/>
+      <c r="H15" s="254"/>
+      <c r="I15" s="255"/>
     </row>
     <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" s="85" t="s">
@@ -17476,15 +17476,15 @@
       <c r="D16" s="86" t="s">
         <v>640</v>
       </c>
-      <c r="E16" s="269" t="s">
+      <c r="E16" s="270" t="s">
         <v>642</v>
       </c>
-      <c r="F16" s="262"/>
-      <c r="G16" s="269" t="s">
+      <c r="F16" s="245"/>
+      <c r="G16" s="270" t="s">
         <v>643</v>
       </c>
-      <c r="H16" s="263"/>
-      <c r="I16" s="264"/>
+      <c r="H16" s="249"/>
+      <c r="I16" s="250"/>
     </row>
     <row r="17" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A17" s="91">
@@ -17499,15 +17499,15 @@
       <c r="D17" s="88" t="s">
         <v>654</v>
       </c>
-      <c r="E17" s="270" t="s">
+      <c r="E17" s="267" t="s">
         <v>652</v>
       </c>
-      <c r="F17" s="262"/>
-      <c r="G17" s="270" t="s">
+      <c r="F17" s="245"/>
+      <c r="G17" s="267" t="s">
         <v>680</v>
       </c>
-      <c r="H17" s="263"/>
-      <c r="I17" s="264"/>
+      <c r="H17" s="249"/>
+      <c r="I17" s="250"/>
     </row>
     <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.3">
       <c r="A18" s="91">
@@ -17522,15 +17522,15 @@
       <c r="D18" s="88" t="s">
         <v>654</v>
       </c>
-      <c r="E18" s="270" t="s">
+      <c r="E18" s="267" t="s">
         <v>652</v>
       </c>
-      <c r="F18" s="262"/>
-      <c r="G18" s="270" t="s">
+      <c r="F18" s="245"/>
+      <c r="G18" s="267" t="s">
         <v>681</v>
       </c>
-      <c r="H18" s="263"/>
-      <c r="I18" s="264"/>
+      <c r="H18" s="249"/>
+      <c r="I18" s="250"/>
     </row>
     <row r="19" spans="1:11" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A19" s="91">
@@ -17545,15 +17545,15 @@
       <c r="D19" s="88" t="s">
         <v>645</v>
       </c>
-      <c r="E19" s="270" t="s">
+      <c r="E19" s="267" t="s">
         <v>683</v>
       </c>
-      <c r="F19" s="262"/>
-      <c r="G19" s="270" t="s">
+      <c r="F19" s="245"/>
+      <c r="G19" s="267" t="s">
         <v>684</v>
       </c>
-      <c r="H19" s="263"/>
-      <c r="I19" s="264"/>
+      <c r="H19" s="249"/>
+      <c r="I19" s="250"/>
       <c r="K19" s="84" t="s">
         <v>646</v>
       </c>
@@ -17565,11 +17565,11 @@
       <c r="B20" s="92"/>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
-      <c r="E20" s="261"/>
-      <c r="F20" s="262"/>
-      <c r="G20" s="261"/>
-      <c r="H20" s="263"/>
-      <c r="I20" s="264"/>
+      <c r="E20" s="244"/>
+      <c r="F20" s="245"/>
+      <c r="G20" s="244"/>
+      <c r="H20" s="249"/>
+      <c r="I20" s="250"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="91">
@@ -17578,11 +17578,11 @@
       <c r="B21" s="92"/>
       <c r="C21" s="92"/>
       <c r="D21" s="92"/>
-      <c r="E21" s="261"/>
-      <c r="F21" s="262"/>
-      <c r="G21" s="261"/>
-      <c r="H21" s="263"/>
-      <c r="I21" s="264"/>
+      <c r="E21" s="244"/>
+      <c r="F21" s="245"/>
+      <c r="G21" s="244"/>
+      <c r="H21" s="249"/>
+      <c r="I21" s="250"/>
       <c r="K21" s="84" t="s">
         <v>685</v>
       </c>
@@ -17594,11 +17594,11 @@
       <c r="B22" s="92"/>
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
-      <c r="E22" s="261"/>
-      <c r="F22" s="262"/>
-      <c r="G22" s="261"/>
-      <c r="H22" s="263"/>
-      <c r="I22" s="264"/>
+      <c r="E22" s="244"/>
+      <c r="F22" s="245"/>
+      <c r="G22" s="244"/>
+      <c r="H22" s="249"/>
+      <c r="I22" s="250"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="91">
@@ -17607,11 +17607,11 @@
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
       <c r="D23" s="92"/>
-      <c r="E23" s="261"/>
-      <c r="F23" s="262"/>
-      <c r="G23" s="261"/>
-      <c r="H23" s="263"/>
-      <c r="I23" s="264"/>
+      <c r="E23" s="244"/>
+      <c r="F23" s="245"/>
+      <c r="G23" s="244"/>
+      <c r="H23" s="249"/>
+      <c r="I23" s="250"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="91">
@@ -17620,11 +17620,11 @@
       <c r="B24" s="92"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
-      <c r="E24" s="261"/>
-      <c r="F24" s="262"/>
-      <c r="G24" s="261"/>
-      <c r="H24" s="263"/>
-      <c r="I24" s="264"/>
+      <c r="E24" s="244"/>
+      <c r="F24" s="245"/>
+      <c r="G24" s="244"/>
+      <c r="H24" s="249"/>
+      <c r="I24" s="250"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="91">
@@ -17633,11 +17633,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="265"/>
-      <c r="F25" s="262"/>
-      <c r="G25" s="265"/>
-      <c r="H25" s="263"/>
-      <c r="I25" s="264"/>
+      <c r="E25" s="246"/>
+      <c r="F25" s="245"/>
+      <c r="G25" s="246"/>
+      <c r="H25" s="249"/>
+      <c r="I25" s="250"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="94">
@@ -17646,10 +17646,10 @@
       <c r="B26" s="95"/>
       <c r="C26" s="95"/>
       <c r="D26" s="95"/>
-      <c r="E26" s="266"/>
+      <c r="E26" s="247"/>
       <c r="F26" s="248"/>
-      <c r="G26" s="266"/>
-      <c r="H26" s="250"/>
+      <c r="G26" s="247"/>
+      <c r="H26" s="251"/>
       <c r="I26" s="252"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18628,14 +18628,16 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="E18:F18"/>
@@ -18648,16 +18650,14 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="G22:I22"/>
-    <mergeCell ref="K6:Q6"/>
-    <mergeCell ref="K7:Q7"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G26:I26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -18688,8 +18688,8 @@
       <c r="A5" s="271" t="s">
         <v>687</v>
       </c>
-      <c r="B5" s="263"/>
-      <c r="C5" s="262"/>
+      <c r="B5" s="249"/>
+      <c r="C5" s="245"/>
     </row>
     <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="101" t="s">
@@ -18748,8 +18748,8 @@
     </row>
     <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="272"/>
-      <c r="B12" s="268"/>
-      <c r="C12" s="268"/>
+      <c r="B12" s="269"/>
+      <c r="C12" s="269"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="109"/>
@@ -19786,7 +19786,7 @@
       <c r="B2" s="273" t="s">
         <v>698</v>
       </c>
-      <c r="C2" s="262"/>
+      <c r="C2" s="245"/>
       <c r="O2" s="84" t="s">
         <v>686</v>
       </c>
@@ -21002,8 +21002,8 @@
       <c r="A3" s="273" t="s">
         <v>731</v>
       </c>
-      <c r="B3" s="263"/>
-      <c r="C3" s="262"/>
+      <c r="B3" s="249"/>
+      <c r="C3" s="245"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="101" t="s">
@@ -21012,7 +21012,7 @@
       <c r="B4" s="271" t="s">
         <v>732</v>
       </c>
-      <c r="C4" s="262"/>
+      <c r="C4" s="245"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="120" t="s">
@@ -21021,7 +21021,7 @@
       <c r="B5" s="274" t="s">
         <v>733</v>
       </c>
-      <c r="C5" s="262"/>
+      <c r="C5" s="245"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="120" t="s">
@@ -21030,7 +21030,7 @@
       <c r="B6" s="274" t="s">
         <v>734</v>
       </c>
-      <c r="C6" s="262"/>
+      <c r="C6" s="245"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="120" t="s">
@@ -21039,7 +21039,7 @@
       <c r="B7" s="274" t="s">
         <v>735</v>
       </c>
-      <c r="C7" s="262"/>
+      <c r="C7" s="245"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="120" t="s">
@@ -21048,13 +21048,13 @@
       <c r="B8" s="274" t="s">
         <v>736</v>
       </c>
-      <c r="C8" s="262"/>
+      <c r="C8" s="245"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B13" s="273" t="s">
         <v>698</v>
       </c>
-      <c r="C13" s="262"/>
+      <c r="C13" s="245"/>
     </row>
     <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B14" s="116" t="s">
@@ -22255,8 +22255,8 @@
       <c r="B2" s="275" t="s">
         <v>737</v>
       </c>
-      <c r="C2" s="245"/>
-      <c r="D2" s="246"/>
+      <c r="C2" s="261"/>
+      <c r="D2" s="262"/>
       <c r="J2" s="84" t="s">
         <v>686</v>
       </c>

</xml_diff>

<commit_message>
Updated name from OPARTGT to SYTGT
</commit_message>
<xml_diff>
--- a/UNDER DEVELOPMENT/OPAR Version 2/JESTER/OPAR v2.0_JOINT_TARGET_LIST_JESTER.xlsx
+++ b/UNDER DEVELOPMENT/OPAR Version 2/JESTER/OPAR v2.0_JOINT_TARGET_LIST_JESTER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\132nd\02 Operations\OPAR\V2\OPAR_BRIEF\UNDER DEVELOPMENT\OPAR Version 2\JESTER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E2EEB4-861D-4DC5-BE4D-A42721B67E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DC0217-3026-4AFC-ADCD-E1AC868DDC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18390" yWindow="2450" windowWidth="17340" windowHeight="14000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="932">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="1044">
   <si>
     <t>OP ACTIVE RESOLVE JOINT TARGET LIST</t>
   </si>
@@ -1877,27 +1877,15 @@
     <t>Backup SDACC Center ( east ).</t>
   </si>
   <si>
-    <t>OPARTGT105</t>
-  </si>
-  <si>
     <t>1st Fighter Aviation Regiment HQ</t>
   </si>
   <si>
-    <t>OPARTGT106</t>
-  </si>
-  <si>
     <t>2nd Fighter Aviation Regiment HQ</t>
   </si>
   <si>
-    <t>OPARTGT107</t>
-  </si>
-  <si>
     <t>4th Fighter Aviation Regiment HQ</t>
   </si>
   <si>
-    <t>OPARTGT108</t>
-  </si>
-  <si>
     <t>5th Assault Aviation Regiment HQ</t>
   </si>
   <si>
@@ -1907,19 +1895,10 @@
     <t>6th Assault Aviation Regiment HQ</t>
   </si>
   <si>
-    <t>OPARTGT110</t>
-  </si>
-  <si>
     <t>7th Bomber Regiment HQ</t>
   </si>
   <si>
-    <t>OPARTGT111</t>
-  </si>
-  <si>
     <t>8th Interceptor Regiment HQ</t>
-  </si>
-  <si>
-    <t>OPARTGT112</t>
   </si>
   <si>
     <t>9th Transport Aviation Regiment HQ</t>
@@ -2423,75 +2402,6 @@
     <t>Current as of: Event start</t>
   </si>
   <si>
-    <t>OPARTGT113</t>
-  </si>
-  <si>
-    <t>OPARTGT114</t>
-  </si>
-  <si>
-    <t>OPARTGT115</t>
-  </si>
-  <si>
-    <t>OPARTGT116</t>
-  </si>
-  <si>
-    <t>OPARTGT117</t>
-  </si>
-  <si>
-    <t>OPARTGT118</t>
-  </si>
-  <si>
-    <t>OPARTGT119</t>
-  </si>
-  <si>
-    <t>OPARTGT120</t>
-  </si>
-  <si>
-    <t>OPARTGT121</t>
-  </si>
-  <si>
-    <t>OPARTGT122</t>
-  </si>
-  <si>
-    <t>OPARTGT123</t>
-  </si>
-  <si>
-    <t>OPARTGT124</t>
-  </si>
-  <si>
-    <t>OPARTGT125</t>
-  </si>
-  <si>
-    <t>OPARTGT126</t>
-  </si>
-  <si>
-    <t>OPARTGT127</t>
-  </si>
-  <si>
-    <t>OPARTGT128</t>
-  </si>
-  <si>
-    <t>OPARTGT129</t>
-  </si>
-  <si>
-    <t>OPARTGT130</t>
-  </si>
-  <si>
-    <t>OPARTGT131</t>
-  </si>
-  <si>
-    <t>OPARTGT132</t>
-  </si>
-  <si>
-    <t>OPARTGT133</t>
-  </si>
-  <si>
-    <t>OPARTGT134</t>
-  </si>
-  <si>
-    <t>OPARTGT135</t>
-  </si>
-  <si>
     <t>Effect of taking out</t>
   </si>
   <si>
@@ -2853,6 +2763,432 @@
   </si>
   <si>
     <t>2301ft</t>
+  </si>
+  <si>
+    <t>Presidential Palace</t>
+  </si>
+  <si>
+    <t>Homs Oil Refinery</t>
+  </si>
+  <si>
+    <t>Hama Ore Processing</t>
+  </si>
+  <si>
+    <t>Al Safira Chemical Weapons Depot</t>
+  </si>
+  <si>
+    <t>SYTGT001</t>
+  </si>
+  <si>
+    <t>SYTGT002</t>
+  </si>
+  <si>
+    <t>SYTGT003</t>
+  </si>
+  <si>
+    <t>SYTGT004</t>
+  </si>
+  <si>
+    <t>SYTGT005</t>
+  </si>
+  <si>
+    <t>SYTGT006</t>
+  </si>
+  <si>
+    <t>SYTGT007</t>
+  </si>
+  <si>
+    <t>SYTGT008</t>
+  </si>
+  <si>
+    <t>SYTGT009</t>
+  </si>
+  <si>
+    <t>SYTGT010</t>
+  </si>
+  <si>
+    <t>SYTGT011</t>
+  </si>
+  <si>
+    <t>SYTGT012</t>
+  </si>
+  <si>
+    <t>SYTGT013</t>
+  </si>
+  <si>
+    <t>SYTGT014</t>
+  </si>
+  <si>
+    <t>SYTGT015</t>
+  </si>
+  <si>
+    <t>SYTGT016</t>
+  </si>
+  <si>
+    <t>SYTGT017</t>
+  </si>
+  <si>
+    <t>SYTGT018</t>
+  </si>
+  <si>
+    <t>SYTGT019</t>
+  </si>
+  <si>
+    <t>SYTGT020</t>
+  </si>
+  <si>
+    <t>SYTGT021</t>
+  </si>
+  <si>
+    <t>SYTGT022</t>
+  </si>
+  <si>
+    <t>SYTGT023</t>
+  </si>
+  <si>
+    <t>SYTGT024</t>
+  </si>
+  <si>
+    <t>SYTGT025</t>
+  </si>
+  <si>
+    <t>SYTGT026</t>
+  </si>
+  <si>
+    <t>SYTGT027</t>
+  </si>
+  <si>
+    <t>SYTGT028</t>
+  </si>
+  <si>
+    <t>SYTGT029</t>
+  </si>
+  <si>
+    <t>SYTGT030</t>
+  </si>
+  <si>
+    <t>SYTGT031</t>
+  </si>
+  <si>
+    <t>SYTGT032</t>
+  </si>
+  <si>
+    <t>SYTGT033</t>
+  </si>
+  <si>
+    <t>SYTGT034</t>
+  </si>
+  <si>
+    <t>SYTGT035</t>
+  </si>
+  <si>
+    <t>SYTGT036</t>
+  </si>
+  <si>
+    <t>SYTGT037</t>
+  </si>
+  <si>
+    <t>SYTGT038</t>
+  </si>
+  <si>
+    <t>SYTGT039</t>
+  </si>
+  <si>
+    <t>SYTGT040</t>
+  </si>
+  <si>
+    <t>SYTGT041</t>
+  </si>
+  <si>
+    <t>SYTGT042</t>
+  </si>
+  <si>
+    <t>SYTGT043</t>
+  </si>
+  <si>
+    <t>SYTGT044</t>
+  </si>
+  <si>
+    <t>SYTGT045</t>
+  </si>
+  <si>
+    <t>SYTGT046</t>
+  </si>
+  <si>
+    <t>SYTGT047</t>
+  </si>
+  <si>
+    <t>SYTGT048</t>
+  </si>
+  <si>
+    <t>SYTGT049</t>
+  </si>
+  <si>
+    <t>SYTGT050</t>
+  </si>
+  <si>
+    <t>SYTGT051</t>
+  </si>
+  <si>
+    <t>SYTGT052</t>
+  </si>
+  <si>
+    <t>SYTGT053</t>
+  </si>
+  <si>
+    <t>SYTGT054</t>
+  </si>
+  <si>
+    <t>SYTGT055</t>
+  </si>
+  <si>
+    <t>SYTGT056</t>
+  </si>
+  <si>
+    <t>SYTGT057</t>
+  </si>
+  <si>
+    <t>SYTGT058</t>
+  </si>
+  <si>
+    <t>SYTGT059</t>
+  </si>
+  <si>
+    <t>SYTGT060</t>
+  </si>
+  <si>
+    <t>SYTGT061</t>
+  </si>
+  <si>
+    <t>SYTGT062</t>
+  </si>
+  <si>
+    <t>SYTGT063</t>
+  </si>
+  <si>
+    <t>SYTGT064</t>
+  </si>
+  <si>
+    <t>SYTGT065</t>
+  </si>
+  <si>
+    <t>SYTGT066</t>
+  </si>
+  <si>
+    <t>SYTGT067</t>
+  </si>
+  <si>
+    <t>SYTGT068</t>
+  </si>
+  <si>
+    <t>SYTGT069</t>
+  </si>
+  <si>
+    <t>SYTGT070</t>
+  </si>
+  <si>
+    <t>SYTGT071</t>
+  </si>
+  <si>
+    <t>SYTGT072</t>
+  </si>
+  <si>
+    <t>SYTGT073</t>
+  </si>
+  <si>
+    <t>SYTGT074</t>
+  </si>
+  <si>
+    <t>SYTGT075</t>
+  </si>
+  <si>
+    <t>SYTGT076</t>
+  </si>
+  <si>
+    <t>SYTGT077</t>
+  </si>
+  <si>
+    <t>SYTGT078</t>
+  </si>
+  <si>
+    <t>SYTGT079</t>
+  </si>
+  <si>
+    <t>SYTGT080</t>
+  </si>
+  <si>
+    <t>SYTGT081</t>
+  </si>
+  <si>
+    <t>SYTGT082</t>
+  </si>
+  <si>
+    <t>SYTGT083</t>
+  </si>
+  <si>
+    <t>SYTGT084</t>
+  </si>
+  <si>
+    <t>SYTGT085</t>
+  </si>
+  <si>
+    <t>SYTGT086</t>
+  </si>
+  <si>
+    <t>SYTGT087</t>
+  </si>
+  <si>
+    <t>SYTGT088</t>
+  </si>
+  <si>
+    <t>SYTGT089</t>
+  </si>
+  <si>
+    <t>SYTGT090</t>
+  </si>
+  <si>
+    <t>SYTGT091</t>
+  </si>
+  <si>
+    <t>SYTGT092</t>
+  </si>
+  <si>
+    <t>SYTGT093</t>
+  </si>
+  <si>
+    <t>SYTGT094</t>
+  </si>
+  <si>
+    <t>SYTGT095</t>
+  </si>
+  <si>
+    <t>SYTGT096</t>
+  </si>
+  <si>
+    <t>SYTGT097</t>
+  </si>
+  <si>
+    <t>SYTGT098</t>
+  </si>
+  <si>
+    <t>SYTGT099</t>
+  </si>
+  <si>
+    <t>SYTGT100</t>
+  </si>
+  <si>
+    <t>SYTGT101</t>
+  </si>
+  <si>
+    <t>SYTGT102</t>
+  </si>
+  <si>
+    <t>SYTGT103</t>
+  </si>
+  <si>
+    <t>SYTGT104</t>
+  </si>
+  <si>
+    <t>SYTGT105</t>
+  </si>
+  <si>
+    <t>SYTGT106</t>
+  </si>
+  <si>
+    <t>SYTGT107</t>
+  </si>
+  <si>
+    <t>SYTGT108</t>
+  </si>
+  <si>
+    <t>SYTGT109</t>
+  </si>
+  <si>
+    <t>SYTGT110</t>
+  </si>
+  <si>
+    <t>SYTGT111</t>
+  </si>
+  <si>
+    <t>SYTGT112</t>
+  </si>
+  <si>
+    <t>SYTGT113</t>
+  </si>
+  <si>
+    <t>SYTGT114</t>
+  </si>
+  <si>
+    <t>SYTGT115</t>
+  </si>
+  <si>
+    <t>SYTGT116</t>
+  </si>
+  <si>
+    <t>SYTGT117</t>
+  </si>
+  <si>
+    <t>SYTGT118</t>
+  </si>
+  <si>
+    <t>SYTGT119</t>
+  </si>
+  <si>
+    <t>SYTGT120</t>
+  </si>
+  <si>
+    <t>SYTGT121</t>
+  </si>
+  <si>
+    <t>SYTGT122</t>
+  </si>
+  <si>
+    <t>SYTGT123</t>
+  </si>
+  <si>
+    <t>SYTGT124</t>
+  </si>
+  <si>
+    <t>SYTGT125</t>
+  </si>
+  <si>
+    <t>SYTGT126</t>
+  </si>
+  <si>
+    <t>SYTGT127</t>
+  </si>
+  <si>
+    <t>SYTGT128</t>
+  </si>
+  <si>
+    <t>SYTGT129</t>
+  </si>
+  <si>
+    <t>SYTGT130</t>
+  </si>
+  <si>
+    <t>SYTGT131</t>
+  </si>
+  <si>
+    <t>SYTGT132</t>
+  </si>
+  <si>
+    <t>SYTGT133</t>
+  </si>
+  <si>
+    <t>SYTGT134</t>
+  </si>
+  <si>
+    <t>SYTGT135</t>
+  </si>
+  <si>
+    <t>SYTGT136</t>
+  </si>
+  <si>
+    <t>SYTGT137</t>
+  </si>
+  <si>
+    <t>SYTGT138</t>
   </si>
 </sst>
 </file>
@@ -4430,6 +4766,32 @@
     <xf numFmtId="0" fontId="43" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="41" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4502,32 +4864,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="18" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="19" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="41" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6363,9 +6699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C131" sqref="C131"/>
+      <selection pane="topRight" activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6383,20 +6719,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="251" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="241"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="215" t="s">
-        <v>787</v>
+        <v>780</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
@@ -6432,12 +6768,12 @@
         <v>8</v>
       </c>
       <c r="I3" s="220" t="s">
-        <v>811</v>
+        <v>781</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="148" t="s">
-        <v>9</v>
+        <v>906</v>
       </c>
       <c r="B4" s="153" t="s">
         <v>10</v>
@@ -6461,7 +6797,7 @@
     </row>
     <row r="5" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="149" t="s">
-        <v>16</v>
+        <v>907</v>
       </c>
       <c r="B5" s="195" t="s">
         <v>17</v>
@@ -6485,7 +6821,7 @@
     </row>
     <row r="6" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="150" t="s">
-        <v>21</v>
+        <v>908</v>
       </c>
       <c r="B6" s="189" t="s">
         <v>22</v>
@@ -6509,7 +6845,7 @@
     </row>
     <row r="7" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="154" t="s">
-        <v>26</v>
+        <v>909</v>
       </c>
       <c r="B7" s="192" t="s">
         <v>27</v>
@@ -6533,7 +6869,7 @@
     </row>
     <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="235" t="s">
-        <v>32</v>
+        <v>910</v>
       </c>
       <c r="B8" s="152" t="s">
         <v>33</v>
@@ -6557,7 +6893,7 @@
     </row>
     <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="236" t="s">
-        <v>39</v>
+        <v>911</v>
       </c>
       <c r="B9" s="156" t="s">
         <v>40</v>
@@ -6581,7 +6917,7 @@
     </row>
     <row r="10" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="235" t="s">
-        <v>46</v>
+        <v>912</v>
       </c>
       <c r="B10" s="237" t="s">
         <v>47</v>
@@ -6605,7 +6941,7 @@
     </row>
     <row r="11" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="236" t="s">
-        <v>53</v>
+        <v>913</v>
       </c>
       <c r="B11" s="238" t="s">
         <v>54</v>
@@ -6629,7 +6965,7 @@
     </row>
     <row r="12" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="235" t="s">
-        <v>59</v>
+        <v>914</v>
       </c>
       <c r="B12" s="237" t="s">
         <v>60</v>
@@ -6653,7 +6989,7 @@
     </row>
     <row r="13" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="236" t="s">
-        <v>64</v>
+        <v>915</v>
       </c>
       <c r="B13" s="238" t="s">
         <v>65</v>
@@ -6677,7 +7013,7 @@
     </row>
     <row r="14" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="235" t="s">
-        <v>69</v>
+        <v>916</v>
       </c>
       <c r="B14" s="237" t="s">
         <v>70</v>
@@ -6701,7 +7037,7 @@
     </row>
     <row r="15" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="236" t="s">
-        <v>75</v>
+        <v>917</v>
       </c>
       <c r="B15" s="238" t="s">
         <v>76</v>
@@ -6725,7 +7061,7 @@
     </row>
     <row r="16" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="235" t="s">
-        <v>80</v>
+        <v>918</v>
       </c>
       <c r="B16" s="237" t="s">
         <v>81</v>
@@ -6749,7 +7085,7 @@
     </row>
     <row r="17" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="236" t="s">
-        <v>86</v>
+        <v>919</v>
       </c>
       <c r="B17" s="238" t="s">
         <v>87</v>
@@ -6773,7 +7109,7 @@
     </row>
     <row r="18" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="235" t="s">
-        <v>91</v>
+        <v>920</v>
       </c>
       <c r="B18" s="237" t="s">
         <v>92</v>
@@ -6797,7 +7133,7 @@
     </row>
     <row r="19" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="236" t="s">
-        <v>97</v>
+        <v>921</v>
       </c>
       <c r="B19" s="238" t="s">
         <v>65</v>
@@ -6821,7 +7157,7 @@
     </row>
     <row r="20" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="235" t="s">
-        <v>103</v>
+        <v>922</v>
       </c>
       <c r="B20" s="237" t="s">
         <v>104</v>
@@ -6845,7 +7181,7 @@
     </row>
     <row r="21" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="149" t="s">
-        <v>109</v>
+        <v>923</v>
       </c>
       <c r="B21" s="156" t="s">
         <v>110</v>
@@ -6887,7 +7223,7 @@
     </row>
     <row r="22" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="150" t="s">
-        <v>116</v>
+        <v>924</v>
       </c>
       <c r="B22" s="189" t="s">
         <v>117</v>
@@ -6912,7 +7248,7 @@
     </row>
     <row r="23" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="149" t="s">
-        <v>123</v>
+        <v>925</v>
       </c>
       <c r="B23" s="201" t="s">
         <v>124</v>
@@ -6937,7 +7273,7 @@
     </row>
     <row r="24" spans="1:26" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="150" t="s">
-        <v>129</v>
+        <v>926</v>
       </c>
       <c r="B24" s="152" t="s">
         <v>130</v>
@@ -6962,7 +7298,7 @@
     </row>
     <row r="25" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="149" t="s">
-        <v>136</v>
+        <v>927</v>
       </c>
       <c r="B25" s="156" t="s">
         <v>137</v>
@@ -6987,7 +7323,7 @@
     </row>
     <row r="26" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="150" t="s">
-        <v>142</v>
+        <v>928</v>
       </c>
       <c r="B26" s="152" t="s">
         <v>143</v>
@@ -7012,7 +7348,7 @@
     </row>
     <row r="27" spans="1:26" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="236" t="s">
-        <v>147</v>
+        <v>929</v>
       </c>
       <c r="B27" s="238" t="s">
         <v>148</v>
@@ -7037,7 +7373,7 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="235" t="s">
-        <v>153</v>
+        <v>930</v>
       </c>
       <c r="B28" s="237" t="s">
         <v>154</v>
@@ -7062,7 +7398,7 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="236" t="s">
-        <v>159</v>
+        <v>931</v>
       </c>
       <c r="B29" s="238" t="s">
         <v>160</v>
@@ -7087,7 +7423,7 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="235" t="s">
-        <v>166</v>
+        <v>932</v>
       </c>
       <c r="B30" s="237" t="s">
         <v>167</v>
@@ -7112,7 +7448,7 @@
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="160" t="s">
-        <v>171</v>
+        <v>933</v>
       </c>
       <c r="B31" s="156" t="s">
         <v>172</v>
@@ -7137,7 +7473,7 @@
     </row>
     <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="158" t="s">
-        <v>177</v>
+        <v>934</v>
       </c>
       <c r="B32" s="152" t="s">
         <v>178</v>
@@ -7162,7 +7498,7 @@
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="160" t="s">
-        <v>183</v>
+        <v>935</v>
       </c>
       <c r="B33" s="156" t="s">
         <v>184</v>
@@ -7187,7 +7523,7 @@
     </row>
     <row r="34" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="158" t="s">
-        <v>190</v>
+        <v>936</v>
       </c>
       <c r="B34" s="152" t="s">
         <v>191</v>
@@ -7212,7 +7548,7 @@
     </row>
     <row r="35" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="160" t="s">
-        <v>196</v>
+        <v>937</v>
       </c>
       <c r="B35" s="156" t="s">
         <v>197</v>
@@ -7236,7 +7572,7 @@
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="158" t="s">
-        <v>201</v>
+        <v>938</v>
       </c>
       <c r="B36" s="152" t="s">
         <v>202</v>
@@ -7260,7 +7596,7 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="154" t="s">
-        <v>207</v>
+        <v>939</v>
       </c>
       <c r="B37" s="156" t="s">
         <v>208</v>
@@ -7284,7 +7620,7 @@
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="164" t="s">
-        <v>214</v>
+        <v>940</v>
       </c>
       <c r="B38" s="152" t="s">
         <v>215</v>
@@ -7308,7 +7644,7 @@
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="160" t="s">
-        <v>220</v>
+        <v>941</v>
       </c>
       <c r="B39" s="156" t="s">
         <v>221</v>
@@ -7333,7 +7669,7 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="158" t="s">
-        <v>228</v>
+        <v>942</v>
       </c>
       <c r="B40" s="152" t="s">
         <v>229</v>
@@ -7357,7 +7693,7 @@
     </row>
     <row r="41" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="160" t="s">
-        <v>233</v>
+        <v>943</v>
       </c>
       <c r="B41" s="156" t="s">
         <v>234</v>
@@ -7381,7 +7717,7 @@
     </row>
     <row r="42" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="164" t="s">
-        <v>237</v>
+        <v>944</v>
       </c>
       <c r="B42" s="167" t="s">
         <v>238</v>
@@ -7405,7 +7741,7 @@
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="154" t="s">
-        <v>243</v>
+        <v>945</v>
       </c>
       <c r="B43" s="156" t="s">
         <v>244</v>
@@ -7429,7 +7765,7 @@
     </row>
     <row r="44" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="164" t="s">
-        <v>249</v>
+        <v>946</v>
       </c>
       <c r="B44" s="152" t="s">
         <v>250</v>
@@ -7453,7 +7789,7 @@
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="160" t="s">
-        <v>255</v>
+        <v>947</v>
       </c>
       <c r="B45" s="156" t="s">
         <v>256</v>
@@ -7477,7 +7813,7 @@
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="158" t="s">
-        <v>260</v>
+        <v>948</v>
       </c>
       <c r="B46" s="152" t="s">
         <v>261</v>
@@ -7501,7 +7837,7 @@
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="160" t="s">
-        <v>266</v>
+        <v>949</v>
       </c>
       <c r="B47" s="156" t="s">
         <v>267</v>
@@ -7525,7 +7861,7 @@
     </row>
     <row r="48" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="158" t="s">
-        <v>272</v>
+        <v>950</v>
       </c>
       <c r="B48" s="152" t="s">
         <v>273</v>
@@ -7549,7 +7885,7 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="160" t="s">
-        <v>277</v>
+        <v>951</v>
       </c>
       <c r="B49" s="156" t="s">
         <v>278</v>
@@ -7573,7 +7909,7 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="158" t="s">
-        <v>283</v>
+        <v>952</v>
       </c>
       <c r="B50" s="152" t="s">
         <v>284</v>
@@ -7597,7 +7933,7 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="160" t="s">
-        <v>289</v>
+        <v>953</v>
       </c>
       <c r="B51" s="156" t="s">
         <v>290</v>
@@ -7621,7 +7957,7 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="158" t="s">
-        <v>294</v>
+        <v>954</v>
       </c>
       <c r="B52" s="152" t="s">
         <v>295</v>
@@ -7639,7 +7975,7 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="160" t="s">
-        <v>297</v>
+        <v>955</v>
       </c>
       <c r="B53" s="156" t="s">
         <v>298</v>
@@ -7663,7 +7999,7 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="158" t="s">
-        <v>301</v>
+        <v>956</v>
       </c>
       <c r="B54" s="152" t="s">
         <v>302</v>
@@ -7687,7 +8023,7 @@
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="160" t="s">
-        <v>306</v>
+        <v>957</v>
       </c>
       <c r="B55" s="156" t="s">
         <v>307</v>
@@ -7711,7 +8047,7 @@
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="164" t="s">
-        <v>311</v>
+        <v>958</v>
       </c>
       <c r="B56" s="152" t="s">
         <v>312</v>
@@ -7735,7 +8071,7 @@
     </row>
     <row r="57" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="160" t="s">
-        <v>316</v>
+        <v>959</v>
       </c>
       <c r="B57" s="156" t="s">
         <v>317</v>
@@ -7759,7 +8095,7 @@
     </row>
     <row r="58" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="158" t="s">
-        <v>321</v>
+        <v>960</v>
       </c>
       <c r="B58" s="152" t="s">
         <v>322</v>
@@ -7783,7 +8119,7 @@
     </row>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="160" t="s">
-        <v>327</v>
+        <v>961</v>
       </c>
       <c r="B59" s="156" t="s">
         <v>328</v>
@@ -7807,7 +8143,7 @@
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="173" t="s">
-        <v>332</v>
+        <v>962</v>
       </c>
       <c r="B60" s="189" t="s">
         <v>333</v>
@@ -7831,7 +8167,7 @@
     </row>
     <row r="61" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="160" t="s">
-        <v>338</v>
+        <v>963</v>
       </c>
       <c r="B61" s="192" t="s">
         <v>339</v>
@@ -7853,12 +8189,12 @@
         <v>344</v>
       </c>
       <c r="I61" s="223" t="s">
-        <v>813</v>
+        <v>783</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="164" t="s">
-        <v>345</v>
+        <v>964</v>
       </c>
       <c r="B62" s="189" t="s">
         <v>346</v>
@@ -7880,12 +8216,12 @@
         <v>350</v>
       </c>
       <c r="I62" s="223" t="s">
-        <v>813</v>
+        <v>783</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="154" t="s">
-        <v>352</v>
+        <v>965</v>
       </c>
       <c r="B63" s="192" t="s">
         <v>353</v>
@@ -7909,7 +8245,7 @@
     </row>
     <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="158" t="s">
-        <v>358</v>
+        <v>966</v>
       </c>
       <c r="B64" s="189" t="s">
         <v>359</v>
@@ -7933,7 +8269,7 @@
     </row>
     <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="160" t="s">
-        <v>364</v>
+        <v>967</v>
       </c>
       <c r="B65" s="156" t="s">
         <v>365</v>
@@ -7957,7 +8293,7 @@
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="158" t="s">
-        <v>370</v>
+        <v>968</v>
       </c>
       <c r="B66" s="152" t="s">
         <v>371</v>
@@ -7981,7 +8317,7 @@
     </row>
     <row r="67" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="160" t="s">
-        <v>377</v>
+        <v>969</v>
       </c>
       <c r="B67" s="156" t="s">
         <v>378</v>
@@ -8005,7 +8341,7 @@
     </row>
     <row r="68" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="158" t="s">
-        <v>384</v>
+        <v>970</v>
       </c>
       <c r="B68" s="152" t="s">
         <v>385</v>
@@ -8029,7 +8365,7 @@
     </row>
     <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="154" t="s">
-        <v>390</v>
+        <v>971</v>
       </c>
       <c r="B69" s="156" t="s">
         <v>391</v>
@@ -8053,7 +8389,7 @@
     </row>
     <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="164" t="s">
-        <v>397</v>
+        <v>972</v>
       </c>
       <c r="B70" s="152" t="s">
         <v>398</v>
@@ -8077,7 +8413,7 @@
     </row>
     <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="160" t="s">
-        <v>402</v>
+        <v>973</v>
       </c>
       <c r="B71" s="156" t="s">
         <v>403</v>
@@ -8101,7 +8437,7 @@
     </row>
     <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="158" t="s">
-        <v>408</v>
+        <v>974</v>
       </c>
       <c r="B72" s="152" t="s">
         <v>409</v>
@@ -8125,7 +8461,7 @@
     </row>
     <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="154" t="s">
-        <v>414</v>
+        <v>975</v>
       </c>
       <c r="B73" s="156" t="s">
         <v>415</v>
@@ -8149,7 +8485,7 @@
     </row>
     <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="158" t="s">
-        <v>420</v>
+        <v>976</v>
       </c>
       <c r="B74" s="152" t="s">
         <v>421</v>
@@ -8173,7 +8509,7 @@
     </row>
     <row r="75" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="154" t="s">
-        <v>423</v>
+        <v>977</v>
       </c>
       <c r="B75" s="156" t="s">
         <v>424</v>
@@ -8197,7 +8533,7 @@
     </row>
     <row r="76" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="164" t="s">
-        <v>429</v>
+        <v>978</v>
       </c>
       <c r="B76" s="152" t="s">
         <v>430</v>
@@ -8221,7 +8557,7 @@
     </row>
     <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="154" t="s">
-        <v>435</v>
+        <v>979</v>
       </c>
       <c r="B77" s="156" t="s">
         <v>436</v>
@@ -8245,7 +8581,7 @@
     </row>
     <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="158" t="s">
-        <v>440</v>
+        <v>980</v>
       </c>
       <c r="B78" s="152" t="s">
         <v>441</v>
@@ -8269,7 +8605,7 @@
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="160" t="s">
-        <v>446</v>
+        <v>981</v>
       </c>
       <c r="B79" s="156" t="s">
         <v>447</v>
@@ -8293,7 +8629,7 @@
     </row>
     <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="158" t="s">
-        <v>452</v>
+        <v>982</v>
       </c>
       <c r="B80" s="152" t="s">
         <v>453</v>
@@ -8317,7 +8653,7 @@
     </row>
     <row r="81" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="160" t="s">
-        <v>458</v>
+        <v>983</v>
       </c>
       <c r="B81" s="156" t="s">
         <v>459</v>
@@ -8341,7 +8677,7 @@
     </row>
     <row r="82" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="158" t="s">
-        <v>463</v>
+        <v>984</v>
       </c>
       <c r="B82" s="152" t="s">
         <v>464</v>
@@ -8365,7 +8701,7 @@
     </row>
     <row r="83" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="160" t="s">
-        <v>469</v>
+        <v>985</v>
       </c>
       <c r="B83" s="156" t="s">
         <v>470</v>
@@ -8387,12 +8723,12 @@
         <v>474</v>
       </c>
       <c r="I83" s="219" t="s">
-        <v>844</v>
+        <v>814</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="158" t="s">
-        <v>475</v>
+        <v>986</v>
       </c>
       <c r="B84" s="189" t="s">
         <v>476</v>
@@ -8414,12 +8750,12 @@
         <v>480</v>
       </c>
       <c r="I84" s="219" t="s">
-        <v>812</v>
+        <v>782</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="160" t="s">
-        <v>481</v>
+        <v>987</v>
       </c>
       <c r="B85" s="156" t="s">
         <v>482</v>
@@ -8443,7 +8779,7 @@
     </row>
     <row r="86" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="158" t="s">
-        <v>488</v>
+        <v>988</v>
       </c>
       <c r="B86" s="152" t="s">
         <v>489</v>
@@ -8467,7 +8803,7 @@
     </row>
     <row r="87" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="160" t="s">
-        <v>495</v>
+        <v>989</v>
       </c>
       <c r="B87" s="156" t="s">
         <v>496</v>
@@ -8491,7 +8827,7 @@
     </row>
     <row r="88" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="175" t="s">
-        <v>502</v>
+        <v>990</v>
       </c>
       <c r="B88" s="152" t="s">
         <v>503</v>
@@ -8515,7 +8851,7 @@
     </row>
     <row r="89" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="154" t="s">
-        <v>507</v>
+        <v>991</v>
       </c>
       <c r="B89" s="156" t="s">
         <v>508</v>
@@ -8539,7 +8875,7 @@
     </row>
     <row r="90" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="158" t="s">
-        <v>513</v>
+        <v>992</v>
       </c>
       <c r="B90" s="152" t="s">
         <v>514</v>
@@ -8563,7 +8899,7 @@
     </row>
     <row r="91" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="154" t="s">
-        <v>519</v>
+        <v>993</v>
       </c>
       <c r="B91" s="156" t="s">
         <v>520</v>
@@ -8587,7 +8923,7 @@
     </row>
     <row r="92" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="164" t="s">
-        <v>525</v>
+        <v>994</v>
       </c>
       <c r="B92" s="152" t="s">
         <v>526</v>
@@ -8611,7 +8947,7 @@
     </row>
     <row r="93" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="160" t="s">
-        <v>531</v>
+        <v>995</v>
       </c>
       <c r="B93" s="156" t="s">
         <v>532</v>
@@ -8635,7 +8971,7 @@
     </row>
     <row r="94" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="158" t="s">
-        <v>537</v>
+        <v>996</v>
       </c>
       <c r="B94" s="189" t="s">
         <v>538</v>
@@ -8659,7 +8995,7 @@
     </row>
     <row r="95" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="160" t="s">
-        <v>543</v>
+        <v>997</v>
       </c>
       <c r="B95" s="156" t="s">
         <v>544</v>
@@ -8683,7 +9019,7 @@
     </row>
     <row r="96" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="158" t="s">
-        <v>547</v>
+        <v>998</v>
       </c>
       <c r="B96" s="152" t="s">
         <v>548</v>
@@ -8707,7 +9043,7 @@
     </row>
     <row r="97" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="154" t="s">
-        <v>553</v>
+        <v>999</v>
       </c>
       <c r="B97" s="156" t="s">
         <v>554</v>
@@ -8729,12 +9065,12 @@
         <v>557</v>
       </c>
       <c r="I97" s="219" t="s">
-        <v>814</v>
+        <v>784</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="158" t="s">
-        <v>558</v>
+        <v>1000</v>
       </c>
       <c r="B98" s="189" t="s">
         <v>559</v>
@@ -8758,7 +9094,7 @@
     </row>
     <row r="99" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="160" t="s">
-        <v>564</v>
+        <v>1001</v>
       </c>
       <c r="B99" s="156" t="s">
         <v>565</v>
@@ -8782,7 +9118,7 @@
     </row>
     <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="158" t="s">
-        <v>570</v>
+        <v>1002</v>
       </c>
       <c r="B100" s="152" t="s">
         <v>571</v>
@@ -8806,7 +9142,7 @@
     </row>
     <row r="101" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="154" t="s">
-        <v>576</v>
+        <v>1003</v>
       </c>
       <c r="B101" s="156" t="s">
         <v>577</v>
@@ -8828,12 +9164,12 @@
         <v>581</v>
       </c>
       <c r="I101" s="219" t="s">
-        <v>843</v>
+        <v>813</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="158" t="s">
-        <v>582</v>
+        <v>1004</v>
       </c>
       <c r="B102" s="152" t="s">
         <v>544</v>
@@ -8857,7 +9193,7 @@
     </row>
     <row r="103" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="160" t="s">
-        <v>587</v>
+        <v>1005</v>
       </c>
       <c r="B103" s="156" t="s">
         <v>588</v>
@@ -8881,7 +9217,7 @@
     </row>
     <row r="104" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="158" t="s">
-        <v>593</v>
+        <v>1006</v>
       </c>
       <c r="B104" s="152" t="s">
         <v>594</v>
@@ -8905,7 +9241,7 @@
     </row>
     <row r="105" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="160" t="s">
-        <v>598</v>
+        <v>1007</v>
       </c>
       <c r="B105" s="192" t="s">
         <v>599</v>
@@ -8929,7 +9265,7 @@
     </row>
     <row r="106" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="164" t="s">
-        <v>603</v>
+        <v>1008</v>
       </c>
       <c r="B106" s="152" t="s">
         <v>604</v>
@@ -8953,7 +9289,7 @@
     </row>
     <row r="107" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="160" t="s">
-        <v>607</v>
+        <v>1009</v>
       </c>
       <c r="B107" s="156" t="s">
         <v>608</v>
@@ -8977,582 +9313,584 @@
     </row>
     <row r="108" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="159" t="s">
-        <v>614</v>
+        <v>1010</v>
       </c>
       <c r="B108" s="152" t="s">
-        <v>815</v>
+        <v>785</v>
       </c>
       <c r="C108" s="165"/>
       <c r="D108" s="162"/>
       <c r="E108" s="172" t="s">
-        <v>816</v>
+        <v>786</v>
       </c>
       <c r="F108" s="172" t="s">
-        <v>817</v>
+        <v>787</v>
       </c>
       <c r="G108" s="151" t="s">
-        <v>818</v>
+        <v>788</v>
       </c>
       <c r="H108" s="176" t="s">
-        <v>824</v>
+        <v>794</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="177" t="s">
-        <v>616</v>
+        <v>1011</v>
       </c>
       <c r="B109" s="156" t="s">
-        <v>819</v>
+        <v>789</v>
       </c>
       <c r="C109" s="178"/>
       <c r="D109" s="179"/>
       <c r="E109" s="180" t="s">
-        <v>820</v>
+        <v>790</v>
       </c>
       <c r="F109" s="180" t="s">
-        <v>821</v>
+        <v>791</v>
       </c>
       <c r="G109" s="181" t="s">
-        <v>822</v>
+        <v>792</v>
       </c>
       <c r="H109" s="182" t="s">
-        <v>823</v>
+        <v>793</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="159" t="s">
-        <v>618</v>
+        <v>1012</v>
       </c>
       <c r="B110" s="152" t="s">
-        <v>825</v>
+        <v>795</v>
       </c>
       <c r="C110" s="165"/>
       <c r="D110" s="162"/>
       <c r="E110" s="172" t="s">
-        <v>826</v>
+        <v>796</v>
       </c>
       <c r="F110" s="172" t="s">
-        <v>827</v>
+        <v>797</v>
       </c>
       <c r="G110" s="151" t="s">
-        <v>828</v>
+        <v>798</v>
       </c>
       <c r="H110" s="176" t="s">
-        <v>825</v>
+        <v>795</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="177" t="s">
-        <v>620</v>
+        <v>1013</v>
       </c>
       <c r="B111" s="224" t="s">
-        <v>829</v>
+        <v>799</v>
       </c>
       <c r="C111" s="225"/>
       <c r="D111" s="225"/>
       <c r="E111" s="226" t="s">
-        <v>830</v>
+        <v>800</v>
       </c>
       <c r="F111" s="226" t="s">
-        <v>831</v>
+        <v>801</v>
       </c>
       <c r="G111" s="225" t="s">
-        <v>838</v>
+        <v>808</v>
       </c>
       <c r="H111" s="226" t="s">
-        <v>832</v>
+        <v>802</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="159" t="s">
-        <v>622</v>
+        <v>1014</v>
       </c>
       <c r="B112" s="227" t="s">
-        <v>833</v>
+        <v>803</v>
       </c>
       <c r="C112" s="228"/>
       <c r="D112" s="228"/>
       <c r="E112" s="229" t="s">
-        <v>835</v>
+        <v>805</v>
       </c>
       <c r="F112" s="229" t="s">
-        <v>836</v>
+        <v>806</v>
       </c>
       <c r="G112" s="230" t="s">
-        <v>837</v>
+        <v>807</v>
       </c>
       <c r="H112" s="229" t="s">
-        <v>834</v>
+        <v>804</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="177" t="s">
-        <v>624</v>
+        <v>1015</v>
       </c>
       <c r="B113" s="183" t="s">
-        <v>839</v>
+        <v>809</v>
       </c>
       <c r="C113" s="184"/>
       <c r="D113" s="184"/>
       <c r="E113" s="185" t="s">
-        <v>840</v>
+        <v>810</v>
       </c>
       <c r="F113" s="185" t="s">
-        <v>841</v>
+        <v>811</v>
       </c>
       <c r="G113" s="185" t="s">
         <v>575</v>
       </c>
       <c r="H113" s="185" t="s">
-        <v>842</v>
+        <v>812</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" s="159" t="s">
-        <v>626</v>
+        <v>1016</v>
       </c>
       <c r="B114" s="186" t="s">
-        <v>845</v>
+        <v>815</v>
       </c>
       <c r="C114" s="187"/>
       <c r="D114" s="187"/>
       <c r="E114" s="185" t="s">
-        <v>847</v>
+        <v>817</v>
       </c>
       <c r="F114" s="188" t="s">
         <v>286</v>
       </c>
       <c r="G114" s="188" t="s">
-        <v>848</v>
+        <v>818</v>
       </c>
       <c r="H114" s="188" t="s">
-        <v>846</v>
+        <v>816</v>
       </c>
       <c r="I114" s="231" t="s">
-        <v>849</v>
+        <v>819</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="177" t="s">
-        <v>628</v>
+        <v>1017</v>
       </c>
       <c r="B115" s="183" t="s">
-        <v>850</v>
+        <v>820</v>
       </c>
       <c r="C115" s="184"/>
       <c r="D115" s="184"/>
       <c r="E115" s="185" t="s">
-        <v>851</v>
+        <v>821</v>
       </c>
       <c r="F115" s="185" t="s">
-        <v>852</v>
+        <v>822</v>
       </c>
       <c r="G115" s="185" t="s">
-        <v>853</v>
+        <v>823</v>
       </c>
       <c r="H115" s="185" t="s">
-        <v>854</v>
+        <v>824</v>
       </c>
       <c r="I115" s="232" t="s">
-        <v>855</v>
+        <v>825</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="159" t="s">
-        <v>788</v>
+        <v>1018</v>
       </c>
       <c r="B116" s="186" t="s">
-        <v>856</v>
+        <v>826</v>
       </c>
       <c r="C116" s="187"/>
       <c r="D116" s="187"/>
       <c r="E116" s="232" t="s">
-        <v>857</v>
+        <v>827</v>
       </c>
       <c r="F116" s="219" t="s">
-        <v>858</v>
+        <v>828</v>
       </c>
       <c r="G116" s="233" t="s">
-        <v>859</v>
+        <v>829</v>
       </c>
       <c r="H116" s="233" t="s">
-        <v>860</v>
+        <v>830</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" s="183" t="s">
-        <v>789</v>
+        <v>1019</v>
       </c>
       <c r="B117" s="183" t="s">
-        <v>862</v>
+        <v>832</v>
       </c>
       <c r="C117" s="184"/>
       <c r="D117" s="184"/>
       <c r="E117" s="185" t="s">
-        <v>863</v>
+        <v>833</v>
       </c>
       <c r="F117" s="185" t="s">
-        <v>864</v>
+        <v>834</v>
       </c>
       <c r="G117" s="185" t="s">
-        <v>865</v>
+        <v>835</v>
       </c>
       <c r="H117" s="185"/>
     </row>
     <row r="118" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" s="159" t="s">
-        <v>790</v>
+        <v>1020</v>
       </c>
       <c r="B118" s="186" t="s">
-        <v>866</v>
+        <v>836</v>
       </c>
       <c r="C118" s="187"/>
       <c r="D118" s="187"/>
       <c r="E118" s="232" t="s">
-        <v>867</v>
+        <v>837</v>
       </c>
       <c r="F118" s="216" t="s">
-        <v>868</v>
+        <v>838</v>
       </c>
       <c r="G118" s="218" t="s">
-        <v>869</v>
+        <v>839</v>
       </c>
       <c r="H118" s="216"/>
     </row>
     <row r="119" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" s="177" t="s">
-        <v>791</v>
+        <v>1021</v>
       </c>
       <c r="B119" s="183" t="s">
-        <v>870</v>
+        <v>840</v>
       </c>
       <c r="C119" s="184"/>
       <c r="D119" s="184"/>
       <c r="E119" s="185" t="s">
-        <v>871</v>
+        <v>841</v>
       </c>
       <c r="F119" s="185" t="s">
-        <v>872</v>
+        <v>842</v>
       </c>
       <c r="G119" s="185" t="s">
-        <v>873</v>
+        <v>843</v>
       </c>
       <c r="H119" s="185" t="s">
-        <v>861</v>
+        <v>831</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" s="159" t="s">
-        <v>792</v>
+        <v>1022</v>
       </c>
       <c r="B120" s="186" t="s">
-        <v>874</v>
+        <v>844</v>
       </c>
       <c r="C120" s="187"/>
       <c r="D120" s="187"/>
       <c r="E120" s="232" t="s">
-        <v>875</v>
+        <v>845</v>
       </c>
       <c r="F120" s="218" t="s">
-        <v>876</v>
+        <v>846</v>
       </c>
       <c r="G120" s="218" t="s">
-        <v>877</v>
+        <v>847</v>
       </c>
       <c r="H120" s="218" t="s">
-        <v>861</v>
+        <v>831</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" s="177" t="s">
-        <v>793</v>
+        <v>1023</v>
       </c>
       <c r="B121" s="183" t="s">
-        <v>878</v>
+        <v>848</v>
       </c>
       <c r="C121" s="184"/>
       <c r="D121" s="184"/>
       <c r="E121" s="232" t="s">
-        <v>879</v>
+        <v>849</v>
       </c>
       <c r="F121" s="218" t="s">
-        <v>880</v>
+        <v>850</v>
       </c>
       <c r="G121" s="218" t="s">
-        <v>881</v>
+        <v>851</v>
       </c>
       <c r="H121" s="218" t="s">
-        <v>861</v>
+        <v>831</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" s="159" t="s">
-        <v>794</v>
+        <v>1024</v>
       </c>
       <c r="B122" s="186" t="s">
-        <v>882</v>
+        <v>852</v>
       </c>
       <c r="C122" s="187"/>
       <c r="D122" s="187"/>
       <c r="E122" s="232" t="s">
-        <v>883</v>
+        <v>853</v>
       </c>
       <c r="F122" s="218" t="s">
-        <v>884</v>
+        <v>854</v>
       </c>
       <c r="G122" s="218" t="s">
-        <v>885</v>
+        <v>855</v>
       </c>
       <c r="H122" s="218" t="s">
-        <v>882</v>
+        <v>852</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="177" t="s">
-        <v>795</v>
+        <v>1025</v>
       </c>
       <c r="B123" s="183" t="s">
-        <v>886</v>
+        <v>856</v>
       </c>
       <c r="C123" s="184"/>
       <c r="D123" s="184"/>
       <c r="E123" s="232" t="s">
-        <v>887</v>
+        <v>857</v>
       </c>
       <c r="F123" s="234" t="s">
         <v>113</v>
       </c>
       <c r="G123" s="234" t="s">
-        <v>888</v>
+        <v>858</v>
       </c>
       <c r="H123" s="234" t="s">
-        <v>889</v>
+        <v>859</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="274" t="s">
-        <v>796</v>
-      </c>
-      <c r="B124" s="275" t="s">
-        <v>890</v>
-      </c>
-      <c r="C124" s="276"/>
-      <c r="D124" s="276"/>
-      <c r="E124" s="277" t="s">
-        <v>891</v>
-      </c>
-      <c r="F124" s="278" t="s">
-        <v>892</v>
-      </c>
-      <c r="G124" s="278" t="s">
-        <v>893</v>
-      </c>
-      <c r="H124" s="278" t="s">
-        <v>890</v>
+      <c r="A124" s="239" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B124" s="240" t="s">
+        <v>860</v>
+      </c>
+      <c r="C124" s="241"/>
+      <c r="D124" s="241"/>
+      <c r="E124" s="242" t="s">
+        <v>861</v>
+      </c>
+      <c r="F124" s="243" t="s">
+        <v>862</v>
+      </c>
+      <c r="G124" s="243" t="s">
+        <v>863</v>
+      </c>
+      <c r="H124" s="243" t="s">
+        <v>860</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" s="177" t="s">
-        <v>797</v>
-      </c>
-      <c r="B125" s="279" t="s">
-        <v>894</v>
-      </c>
-      <c r="C125" s="280"/>
-      <c r="D125" s="281"/>
-      <c r="E125" s="277" t="s">
-        <v>895</v>
-      </c>
-      <c r="F125" s="278" t="s">
-        <v>896</v>
-      </c>
-      <c r="G125" s="279" t="s">
-        <v>897</v>
-      </c>
-      <c r="H125" s="278" t="s">
-        <v>894</v>
+        <v>1027</v>
+      </c>
+      <c r="B125" s="244" t="s">
+        <v>864</v>
+      </c>
+      <c r="C125" s="245"/>
+      <c r="D125" s="246"/>
+      <c r="E125" s="242" t="s">
+        <v>865</v>
+      </c>
+      <c r="F125" s="243" t="s">
+        <v>866</v>
+      </c>
+      <c r="G125" s="244" t="s">
+        <v>867</v>
+      </c>
+      <c r="H125" s="243" t="s">
+        <v>864</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" s="159" t="s">
-        <v>798</v>
-      </c>
-      <c r="B126" s="279" t="s">
-        <v>898</v>
-      </c>
-      <c r="C126" s="280"/>
-      <c r="D126" s="281"/>
-      <c r="E126" s="277" t="s">
-        <v>899</v>
-      </c>
-      <c r="F126" s="278" t="s">
-        <v>900</v>
-      </c>
-      <c r="G126" s="278" t="s">
-        <v>901</v>
-      </c>
-      <c r="H126" s="278" t="s">
-        <v>902</v>
+        <v>1028</v>
+      </c>
+      <c r="B126" s="244" t="s">
+        <v>868</v>
+      </c>
+      <c r="C126" s="245"/>
+      <c r="D126" s="246"/>
+      <c r="E126" s="242" t="s">
+        <v>869</v>
+      </c>
+      <c r="F126" s="243" t="s">
+        <v>870</v>
+      </c>
+      <c r="G126" s="243" t="s">
+        <v>871</v>
+      </c>
+      <c r="H126" s="243" t="s">
+        <v>872</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" s="177" t="s">
-        <v>799</v>
-      </c>
-      <c r="B127" s="282" t="s">
-        <v>914</v>
-      </c>
-      <c r="C127" s="283"/>
-      <c r="D127" s="281"/>
-      <c r="E127" s="277" t="s">
-        <v>904</v>
-      </c>
-      <c r="F127" s="278" t="s">
-        <v>905</v>
-      </c>
-      <c r="G127" s="281" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B127" s="247" t="s">
+        <v>884</v>
+      </c>
+      <c r="C127" s="248"/>
+      <c r="D127" s="246"/>
+      <c r="E127" s="242" t="s">
+        <v>874</v>
+      </c>
+      <c r="F127" s="243" t="s">
+        <v>875</v>
+      </c>
+      <c r="G127" s="246" t="s">
         <v>612</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" s="159" t="s">
-        <v>800</v>
-      </c>
-      <c r="B128" s="282" t="s">
-        <v>909</v>
-      </c>
-      <c r="C128" s="283"/>
-      <c r="D128" s="281"/>
-      <c r="E128" s="277" t="s">
-        <v>906</v>
-      </c>
-      <c r="F128" s="278" t="s">
-        <v>907</v>
-      </c>
-      <c r="G128" s="281" t="s">
-        <v>908</v>
+        <v>1030</v>
+      </c>
+      <c r="B128" s="247" t="s">
+        <v>879</v>
+      </c>
+      <c r="C128" s="248"/>
+      <c r="D128" s="246"/>
+      <c r="E128" s="242" t="s">
+        <v>876</v>
+      </c>
+      <c r="F128" s="243" t="s">
+        <v>877</v>
+      </c>
+      <c r="G128" s="246" t="s">
+        <v>878</v>
       </c>
     </row>
     <row r="129" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" s="177" t="s">
-        <v>801</v>
-      </c>
-      <c r="B129" s="282" t="s">
-        <v>910</v>
-      </c>
-      <c r="C129" s="283"/>
-      <c r="D129" s="281"/>
-      <c r="E129" s="277" t="s">
-        <v>911</v>
-      </c>
-      <c r="F129" s="278" t="s">
-        <v>912</v>
-      </c>
-      <c r="G129" s="281" t="s">
-        <v>913</v>
+        <v>1031</v>
+      </c>
+      <c r="B129" s="247" t="s">
+        <v>880</v>
+      </c>
+      <c r="C129" s="248"/>
+      <c r="D129" s="246"/>
+      <c r="E129" s="242" t="s">
+        <v>881</v>
+      </c>
+      <c r="F129" s="243" t="s">
+        <v>882</v>
+      </c>
+      <c r="G129" s="246" t="s">
+        <v>883</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" s="177" t="s">
-        <v>802</v>
-      </c>
-      <c r="B130" s="282" t="s">
-        <v>903</v>
+        <v>1032</v>
+      </c>
+      <c r="B130" s="247" t="s">
+        <v>873</v>
       </c>
       <c r="C130" s="77"/>
       <c r="D130" s="78"/>
-      <c r="E130" s="277" t="s">
-        <v>915</v>
-      </c>
-      <c r="F130" s="278" t="s">
-        <v>916</v>
+      <c r="E130" s="242" t="s">
+        <v>885</v>
+      </c>
+      <c r="F130" s="243" t="s">
+        <v>886</v>
       </c>
       <c r="G130" s="78" t="s">
-        <v>901</v>
+        <v>871</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" s="159" t="s">
-        <v>803</v>
-      </c>
-      <c r="B131" s="282" t="s">
-        <v>917</v>
-      </c>
-      <c r="C131" s="283"/>
-      <c r="D131" s="281"/>
-      <c r="E131" s="277" t="s">
-        <v>918</v>
-      </c>
-      <c r="F131" s="278" t="s">
-        <v>919</v>
-      </c>
-      <c r="G131" s="281" t="s">
-        <v>920</v>
+        <v>1033</v>
+      </c>
+      <c r="B131" s="247" t="s">
+        <v>887</v>
+      </c>
+      <c r="C131" s="248"/>
+      <c r="D131" s="246"/>
+      <c r="E131" s="242" t="s">
+        <v>888</v>
+      </c>
+      <c r="F131" s="243" t="s">
+        <v>889</v>
+      </c>
+      <c r="G131" s="246" t="s">
+        <v>890</v>
       </c>
     </row>
     <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" s="177" t="s">
-        <v>804</v>
-      </c>
-      <c r="B132" s="282" t="s">
-        <v>917</v>
-      </c>
-      <c r="C132" s="283"/>
-      <c r="D132" s="281"/>
-      <c r="E132" s="277" t="s">
-        <v>921</v>
-      </c>
-      <c r="F132" s="278" t="s">
-        <v>922</v>
-      </c>
-      <c r="G132" s="281" t="s">
-        <v>923</v>
+        <v>1034</v>
+      </c>
+      <c r="B132" s="247" t="s">
+        <v>887</v>
+      </c>
+      <c r="C132" s="248"/>
+      <c r="D132" s="246"/>
+      <c r="E132" s="242" t="s">
+        <v>891</v>
+      </c>
+      <c r="F132" s="243" t="s">
+        <v>892</v>
+      </c>
+      <c r="G132" s="246" t="s">
+        <v>893</v>
       </c>
     </row>
     <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A133" s="274" t="s">
-        <v>805</v>
-      </c>
-      <c r="B133" s="284" t="s">
-        <v>924</v>
-      </c>
-      <c r="C133" s="280"/>
-      <c r="D133" s="281"/>
-      <c r="E133" s="277" t="s">
-        <v>925</v>
-      </c>
-      <c r="F133" s="278" t="s">
-        <v>929</v>
-      </c>
-      <c r="G133" s="281" t="s">
-        <v>930</v>
+      <c r="A133" s="239" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B133" s="249" t="s">
+        <v>894</v>
+      </c>
+      <c r="C133" s="245"/>
+      <c r="D133" s="246"/>
+      <c r="E133" s="242" t="s">
+        <v>895</v>
+      </c>
+      <c r="F133" s="243" t="s">
+        <v>899</v>
+      </c>
+      <c r="G133" s="246" t="s">
+        <v>900</v>
       </c>
       <c r="H133" s="216"/>
     </row>
     <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A134" s="285" t="s">
-        <v>806</v>
-      </c>
-      <c r="B134" s="282" t="s">
-        <v>926</v>
-      </c>
-      <c r="C134" s="283"/>
-      <c r="D134" s="281"/>
-      <c r="E134" s="277" t="s">
-        <v>927</v>
-      </c>
-      <c r="F134" s="278" t="s">
-        <v>928</v>
-      </c>
-      <c r="G134" s="281" t="s">
-        <v>931</v>
+      <c r="A134" s="250" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B134" s="247" t="s">
+        <v>896</v>
+      </c>
+      <c r="C134" s="248"/>
+      <c r="D134" s="246"/>
+      <c r="E134" s="242" t="s">
+        <v>897</v>
+      </c>
+      <c r="F134" s="243" t="s">
+        <v>898</v>
+      </c>
+      <c r="G134" s="246" t="s">
+        <v>901</v>
       </c>
     </row>
     <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="159" t="s">
-        <v>807</v>
-      </c>
-      <c r="B135" s="76"/>
+        <v>1037</v>
+      </c>
+      <c r="B135" s="76" t="s">
+        <v>902</v>
+      </c>
       <c r="C135" s="77"/>
       <c r="D135" s="78"/>
       <c r="E135" s="79"/>
@@ -9561,9 +9899,11 @@
     </row>
     <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="177" t="s">
-        <v>808</v>
-      </c>
-      <c r="B136" s="216"/>
+        <v>1038</v>
+      </c>
+      <c r="B136" s="247" t="s">
+        <v>903</v>
+      </c>
       <c r="C136" s="217"/>
       <c r="D136" s="78"/>
       <c r="E136" s="216"/>
@@ -9573,9 +9913,11 @@
     </row>
     <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="177" t="s">
-        <v>809</v>
-      </c>
-      <c r="B137" s="76"/>
+        <v>1039</v>
+      </c>
+      <c r="B137" s="76" t="s">
+        <v>904</v>
+      </c>
       <c r="C137" s="77"/>
       <c r="D137" s="78"/>
       <c r="E137" s="79"/>
@@ -9584,9 +9926,11 @@
     </row>
     <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="159" t="s">
-        <v>810</v>
-      </c>
-      <c r="B138" s="76"/>
+        <v>1040</v>
+      </c>
+      <c r="B138" s="76" t="s">
+        <v>905</v>
+      </c>
       <c r="C138" s="77"/>
       <c r="D138" s="78"/>
       <c r="E138" s="79"/>
@@ -9594,7 +9938,9 @@
       <c r="G138" s="78"/>
     </row>
     <row r="139" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="76"/>
+      <c r="A139" s="76" t="s">
+        <v>1041</v>
+      </c>
       <c r="B139" s="76"/>
       <c r="C139" s="77"/>
       <c r="D139" s="78"/>
@@ -9603,7 +9949,9 @@
       <c r="G139" s="78"/>
     </row>
     <row r="140" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="76"/>
+      <c r="A140" s="76" t="s">
+        <v>1042</v>
+      </c>
       <c r="B140" s="76"/>
       <c r="C140" s="77"/>
       <c r="D140" s="78"/>
@@ -9612,7 +9960,9 @@
       <c r="G140" s="78"/>
     </row>
     <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="76"/>
+      <c r="A141" s="76" t="s">
+        <v>1043</v>
+      </c>
       <c r="B141" s="76"/>
       <c r="C141" s="77"/>
       <c r="D141" s="78"/>
@@ -9650,7 +10000,7 @@
     <row r="145" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="76"/>
       <c r="B145" s="152" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C145" s="77"/>
       <c r="D145" s="78"/>
@@ -9661,7 +10011,7 @@
     <row r="146" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="76"/>
       <c r="B146" s="156" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="C146" s="77"/>
       <c r="D146" s="78"/>
@@ -9672,7 +10022,7 @@
     <row r="147" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="76"/>
       <c r="B147" s="152" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C147" s="77"/>
       <c r="D147" s="78"/>
@@ -9683,7 +10033,7 @@
     <row r="148" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" s="76"/>
       <c r="B148" s="183" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="C148" s="77"/>
       <c r="D148" s="78"/>
@@ -9694,7 +10044,7 @@
     <row r="149" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" s="76"/>
       <c r="B149" s="186" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C149" s="77"/>
       <c r="D149" s="78"/>
@@ -9705,7 +10055,7 @@
     <row r="150" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="76"/>
       <c r="B150" s="183" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="C150" s="77"/>
       <c r="D150" s="78"/>
@@ -9716,7 +10066,7 @@
     <row r="151" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="76"/>
       <c r="B151" s="186" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="C151" s="77"/>
       <c r="D151" s="78"/>
@@ -9727,7 +10077,7 @@
     <row r="152" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="76"/>
       <c r="B152" s="183" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="C152" s="77"/>
       <c r="D152" s="78"/>
@@ -15992,37 +16342,37 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A21" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A22" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A23" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A25" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A26" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A38" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A42" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A43" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A44" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="A56" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A60" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="A62" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="A63" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="A69" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A70" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A73" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A75" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A76" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A77" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A89" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A91" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A92" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A97" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A101" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A106" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A4" r:id="rId1" display="OPARTGT001" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" display="OPARTGT002" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A6" r:id="rId3" display="OPARTGT003" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A7" r:id="rId4" display="OPARTGT004" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A21" r:id="rId5" display="OPARTGT018" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A22" r:id="rId6" display="OPARTGT019" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A23" r:id="rId7" display="OPARTGT020" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A24" r:id="rId8" display="OPARTGT021" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A25" r:id="rId9" display="OPARTGT022" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A26" r:id="rId10" display="OPARTGT023" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A37" r:id="rId11" display="OPARTGT034" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A38" r:id="rId12" display="OPARTGT035" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A42" r:id="rId13" display="OPARTGT039" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A43" r:id="rId14" display="OPARTGT040" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A44" r:id="rId15" display="OPARTGT041" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A56" r:id="rId16" display="OPARTGT053" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A60" r:id="rId17" display="OPARTGT057" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A62" r:id="rId18" display="OPARTGT059" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A63" r:id="rId19" display="OPARTGT060" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A69" r:id="rId20" display="OPARTGT066" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A70" r:id="rId21" display="OPARTGT067" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A73" r:id="rId22" display="OPARTGT070" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A75" r:id="rId23" display="OPARTGT072" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A76" r:id="rId24" display="OPARTGT073" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A77" r:id="rId25" display="OPARTGT074" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A89" r:id="rId26" display="OPARTGT086" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A91" r:id="rId27" display="OPARTGT088" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A92" r:id="rId28" display="OPARTGT089" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A97" r:id="rId29" display="OPARTGT094" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A101" r:id="rId30" display="OPARTGT098" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A106" r:id="rId31" display="OPARTGT103" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
   </hyperlinks>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId32"/>
@@ -16053,65 +16403,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="242" t="s">
-        <v>630</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="243"/>
-      <c r="I1" s="244"/>
+      <c r="A1" s="254" t="s">
+        <v>623</v>
+      </c>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="256"/>
     </row>
     <row r="2" spans="1:11" ht="14" x14ac:dyDescent="0.3">
-      <c r="A2" s="245" t="s">
-        <v>631</v>
-      </c>
-      <c r="B2" s="246"/>
+      <c r="A2" s="257" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2" s="258"/>
       <c r="C2" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="247" t="s">
-        <v>632</v>
-      </c>
-      <c r="E2" s="248"/>
-      <c r="F2" s="248"/>
-      <c r="G2" s="246"/>
-      <c r="H2" s="249"/>
-      <c r="I2" s="250"/>
+      <c r="D2" s="259" t="s">
+        <v>625</v>
+      </c>
+      <c r="E2" s="260"/>
+      <c r="F2" s="260"/>
+      <c r="G2" s="258"/>
+      <c r="H2" s="261"/>
+      <c r="I2" s="262"/>
     </row>
     <row r="3" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="K3" s="84" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="251" t="s">
-        <v>634</v>
-      </c>
-      <c r="B4" s="243"/>
-      <c r="C4" s="243"/>
-      <c r="D4" s="243"/>
-      <c r="E4" s="243"/>
-      <c r="F4" s="243"/>
-      <c r="G4" s="243"/>
-      <c r="H4" s="243"/>
-      <c r="I4" s="244"/>
+      <c r="A4" s="263" t="s">
+        <v>627</v>
+      </c>
+      <c r="B4" s="255"/>
+      <c r="C4" s="255"/>
+      <c r="D4" s="255"/>
+      <c r="E4" s="255"/>
+      <c r="F4" s="255"/>
+      <c r="G4" s="255"/>
+      <c r="H4" s="255"/>
+      <c r="I4" s="256"/>
     </row>
     <row r="5" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="85" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="B5" s="86" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="C5" s="86" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="E5" s="86" t="s">
         <v>5</v>
@@ -16123,10 +16473,10 @@
         <v>7</v>
       </c>
       <c r="H5" s="86" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="14" x14ac:dyDescent="0.3">
@@ -16245,40 +16595,40 @@
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="252" t="s">
-        <v>641</v>
-      </c>
-      <c r="B15" s="253"/>
-      <c r="C15" s="253"/>
-      <c r="D15" s="253"/>
-      <c r="E15" s="253"/>
-      <c r="F15" s="253"/>
-      <c r="G15" s="253"/>
-      <c r="H15" s="253"/>
-      <c r="I15" s="254"/>
+      <c r="A15" s="264" t="s">
+        <v>634</v>
+      </c>
+      <c r="B15" s="265"/>
+      <c r="C15" s="265"/>
+      <c r="D15" s="265"/>
+      <c r="E15" s="265"/>
+      <c r="F15" s="265"/>
+      <c r="G15" s="265"/>
+      <c r="H15" s="265"/>
+      <c r="I15" s="266"/>
     </row>
     <row r="16" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" s="89" t="s">
+        <v>628</v>
+      </c>
+      <c r="B16" s="90" t="s">
+        <v>631</v>
+      </c>
+      <c r="C16" s="90" t="s">
+        <v>632</v>
+      </c>
+      <c r="D16" s="90" t="s">
+        <v>633</v>
+      </c>
+      <c r="E16" s="267" t="s">
         <v>635</v>
       </c>
-      <c r="B16" s="90" t="s">
-        <v>638</v>
-      </c>
-      <c r="C16" s="90" t="s">
-        <v>639</v>
-      </c>
-      <c r="D16" s="90" t="s">
-        <v>640</v>
-      </c>
-      <c r="E16" s="255" t="s">
-        <v>642</v>
-      </c>
-      <c r="F16" s="258"/>
-      <c r="G16" s="255" t="s">
-        <v>643</v>
-      </c>
-      <c r="H16" s="256"/>
-      <c r="I16" s="257"/>
+      <c r="F16" s="270"/>
+      <c r="G16" s="267" t="s">
+        <v>636</v>
+      </c>
+      <c r="H16" s="268"/>
+      <c r="I16" s="269"/>
     </row>
     <row r="17" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="91">
@@ -16287,13 +16637,13 @@
       <c r="B17" s="92"/>
       <c r="C17" s="92"/>
       <c r="D17" s="92"/>
-      <c r="E17" s="259"/>
-      <c r="F17" s="260"/>
-      <c r="G17" s="259"/>
-      <c r="H17" s="261"/>
-      <c r="I17" s="262"/>
+      <c r="E17" s="271"/>
+      <c r="F17" s="272"/>
+      <c r="G17" s="271"/>
+      <c r="H17" s="273"/>
+      <c r="I17" s="274"/>
       <c r="K17" s="84" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -16303,11 +16653,11 @@
       <c r="B18" s="92"/>
       <c r="C18" s="92"/>
       <c r="D18" s="92"/>
-      <c r="E18" s="259"/>
-      <c r="F18" s="260"/>
-      <c r="G18" s="259"/>
-      <c r="H18" s="261"/>
-      <c r="I18" s="262"/>
+      <c r="E18" s="271"/>
+      <c r="F18" s="272"/>
+      <c r="G18" s="271"/>
+      <c r="H18" s="273"/>
+      <c r="I18" s="274"/>
     </row>
     <row r="19" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="91">
@@ -16316,11 +16666,11 @@
       <c r="B19" s="92"/>
       <c r="C19" s="92"/>
       <c r="D19" s="92"/>
-      <c r="E19" s="259"/>
-      <c r="F19" s="260"/>
-      <c r="G19" s="259"/>
-      <c r="H19" s="261"/>
-      <c r="I19" s="262"/>
+      <c r="E19" s="271"/>
+      <c r="F19" s="272"/>
+      <c r="G19" s="271"/>
+      <c r="H19" s="273"/>
+      <c r="I19" s="274"/>
     </row>
     <row r="20" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="91">
@@ -16329,11 +16679,11 @@
       <c r="B20" s="92"/>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
-      <c r="E20" s="259"/>
-      <c r="F20" s="260"/>
-      <c r="G20" s="259"/>
-      <c r="H20" s="261"/>
-      <c r="I20" s="262"/>
+      <c r="E20" s="271"/>
+      <c r="F20" s="272"/>
+      <c r="G20" s="271"/>
+      <c r="H20" s="273"/>
+      <c r="I20" s="274"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="91">
@@ -16342,11 +16692,11 @@
       <c r="B21" s="92"/>
       <c r="C21" s="92"/>
       <c r="D21" s="92"/>
-      <c r="E21" s="259"/>
-      <c r="F21" s="260"/>
-      <c r="G21" s="259"/>
-      <c r="H21" s="261"/>
-      <c r="I21" s="262"/>
+      <c r="E21" s="271"/>
+      <c r="F21" s="272"/>
+      <c r="G21" s="271"/>
+      <c r="H21" s="273"/>
+      <c r="I21" s="274"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="91">
@@ -16355,11 +16705,11 @@
       <c r="B22" s="92"/>
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
-      <c r="E22" s="259"/>
-      <c r="F22" s="260"/>
-      <c r="G22" s="259"/>
-      <c r="H22" s="261"/>
-      <c r="I22" s="262"/>
+      <c r="E22" s="271"/>
+      <c r="F22" s="272"/>
+      <c r="G22" s="271"/>
+      <c r="H22" s="273"/>
+      <c r="I22" s="274"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="91">
@@ -16368,11 +16718,11 @@
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
       <c r="D23" s="92"/>
-      <c r="E23" s="259"/>
-      <c r="F23" s="260"/>
-      <c r="G23" s="259"/>
-      <c r="H23" s="261"/>
-      <c r="I23" s="262"/>
+      <c r="E23" s="271"/>
+      <c r="F23" s="272"/>
+      <c r="G23" s="271"/>
+      <c r="H23" s="273"/>
+      <c r="I23" s="274"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="91">
@@ -16381,11 +16731,11 @@
       <c r="B24" s="92"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
-      <c r="E24" s="259"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="259"/>
-      <c r="H24" s="261"/>
-      <c r="I24" s="262"/>
+      <c r="E24" s="271"/>
+      <c r="F24" s="272"/>
+      <c r="G24" s="271"/>
+      <c r="H24" s="273"/>
+      <c r="I24" s="274"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="91">
@@ -16394,11 +16744,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="263"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="263"/>
-      <c r="H25" s="261"/>
-      <c r="I25" s="262"/>
+      <c r="E25" s="275"/>
+      <c r="F25" s="272"/>
+      <c r="G25" s="275"/>
+      <c r="H25" s="273"/>
+      <c r="I25" s="274"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="94">
@@ -16407,11 +16757,11 @@
       <c r="B26" s="95"/>
       <c r="C26" s="95"/>
       <c r="D26" s="95"/>
-      <c r="E26" s="264"/>
-      <c r="F26" s="246"/>
-      <c r="G26" s="264"/>
-      <c r="H26" s="248"/>
-      <c r="I26" s="250"/>
+      <c r="E26" s="276"/>
+      <c r="F26" s="258"/>
+      <c r="G26" s="276"/>
+      <c r="H26" s="260"/>
+      <c r="I26" s="262"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -17447,62 +17797,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="242" t="s">
-        <v>630</v>
-      </c>
-      <c r="B1" s="243"/>
-      <c r="C1" s="243"/>
-      <c r="D1" s="243"/>
-      <c r="E1" s="243"/>
-      <c r="F1" s="243"/>
-      <c r="G1" s="243"/>
-      <c r="H1" s="243"/>
-      <c r="I1" s="244"/>
+      <c r="A1" s="254" t="s">
+        <v>623</v>
+      </c>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="256"/>
     </row>
     <row r="2" spans="1:17" ht="14" x14ac:dyDescent="0.3">
-      <c r="A2" s="245" t="s">
-        <v>631</v>
-      </c>
-      <c r="B2" s="246"/>
+      <c r="A2" s="257" t="s">
+        <v>624</v>
+      </c>
+      <c r="B2" s="258"/>
       <c r="C2" s="100" t="s">
-        <v>655</v>
-      </c>
-      <c r="D2" s="247" t="s">
-        <v>632</v>
-      </c>
-      <c r="E2" s="248"/>
-      <c r="F2" s="248"/>
-      <c r="G2" s="246"/>
-      <c r="H2" s="249" t="s">
-        <v>656</v>
-      </c>
-      <c r="I2" s="250"/>
+        <v>648</v>
+      </c>
+      <c r="D2" s="259" t="s">
+        <v>625</v>
+      </c>
+      <c r="E2" s="260"/>
+      <c r="F2" s="260"/>
+      <c r="G2" s="258"/>
+      <c r="H2" s="261" t="s">
+        <v>649</v>
+      </c>
+      <c r="I2" s="262"/>
     </row>
     <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="251" t="s">
-        <v>634</v>
-      </c>
-      <c r="B4" s="243"/>
-      <c r="C4" s="243"/>
-      <c r="D4" s="243"/>
-      <c r="E4" s="243"/>
-      <c r="F4" s="243"/>
-      <c r="G4" s="243"/>
-      <c r="H4" s="243"/>
-      <c r="I4" s="244"/>
+      <c r="A4" s="263" t="s">
+        <v>627</v>
+      </c>
+      <c r="B4" s="255"/>
+      <c r="C4" s="255"/>
+      <c r="D4" s="255"/>
+      <c r="E4" s="255"/>
+      <c r="F4" s="255"/>
+      <c r="G4" s="255"/>
+      <c r="H4" s="255"/>
+      <c r="I4" s="256"/>
     </row>
     <row r="5" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="85" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="B5" s="86" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="C5" s="86" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="E5" s="86" t="s">
         <v>5</v>
@@ -17514,13 +17864,13 @@
         <v>7</v>
       </c>
       <c r="H5" s="86" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="I5" s="87" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="K5" s="84" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="31" x14ac:dyDescent="0.3">
@@ -17528,104 +17878,104 @@
         <v>1</v>
       </c>
       <c r="B6" s="88" t="s">
+        <v>650</v>
+      </c>
+      <c r="C6" s="88" t="s">
+        <v>651</v>
+      </c>
+      <c r="D6" s="88" t="s">
+        <v>652</v>
+      </c>
+      <c r="E6" s="88" t="s">
+        <v>653</v>
+      </c>
+      <c r="F6" s="88" t="s">
+        <v>654</v>
+      </c>
+      <c r="G6" s="88" t="s">
+        <v>655</v>
+      </c>
+      <c r="H6" s="88" t="s">
+        <v>656</v>
+      </c>
+      <c r="I6" s="97" t="s">
         <v>657</v>
       </c>
-      <c r="C6" s="88" t="s">
+      <c r="K6" s="277" t="s">
         <v>658</v>
       </c>
-      <c r="D6" s="88" t="s">
-        <v>659</v>
-      </c>
-      <c r="E6" s="88" t="s">
-        <v>660</v>
-      </c>
-      <c r="F6" s="88" t="s">
-        <v>661</v>
-      </c>
-      <c r="G6" s="88" t="s">
-        <v>662</v>
-      </c>
-      <c r="H6" s="88" t="s">
-        <v>663</v>
-      </c>
-      <c r="I6" s="97" t="s">
-        <v>664</v>
-      </c>
-      <c r="K6" s="265" t="s">
-        <v>665</v>
-      </c>
-      <c r="L6" s="266"/>
-      <c r="M6" s="266"/>
-      <c r="N6" s="266"/>
-      <c r="O6" s="266"/>
-      <c r="P6" s="266"/>
-      <c r="Q6" s="266"/>
+      <c r="L6" s="278"/>
+      <c r="M6" s="278"/>
+      <c r="N6" s="278"/>
+      <c r="O6" s="278"/>
+      <c r="P6" s="278"/>
+      <c r="Q6" s="278"/>
     </row>
     <row r="7" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="96">
         <v>2</v>
       </c>
       <c r="B7" s="88" t="s">
+        <v>659</v>
+      </c>
+      <c r="C7" s="88" t="s">
+        <v>660</v>
+      </c>
+      <c r="D7" s="88" t="s">
+        <v>661</v>
+      </c>
+      <c r="E7" s="88" t="s">
+        <v>662</v>
+      </c>
+      <c r="F7" s="88" t="s">
+        <v>663</v>
+      </c>
+      <c r="G7" s="88" t="s">
+        <v>664</v>
+      </c>
+      <c r="H7" s="88" t="s">
+        <v>644</v>
+      </c>
+      <c r="I7" s="97" t="s">
+        <v>665</v>
+      </c>
+      <c r="K7" s="277" t="s">
         <v>666</v>
       </c>
-      <c r="C7" s="88" t="s">
-        <v>667</v>
-      </c>
-      <c r="D7" s="88" t="s">
-        <v>668</v>
-      </c>
-      <c r="E7" s="88" t="s">
-        <v>669</v>
-      </c>
-      <c r="F7" s="88" t="s">
-        <v>670</v>
-      </c>
-      <c r="G7" s="88" t="s">
-        <v>671</v>
-      </c>
-      <c r="H7" s="88" t="s">
-        <v>651</v>
-      </c>
-      <c r="I7" s="97" t="s">
-        <v>672</v>
-      </c>
-      <c r="K7" s="265" t="s">
-        <v>673</v>
-      </c>
-      <c r="L7" s="266"/>
-      <c r="M7" s="266"/>
-      <c r="N7" s="266"/>
-      <c r="O7" s="266"/>
-      <c r="P7" s="266"/>
-      <c r="Q7" s="266"/>
+      <c r="L7" s="278"/>
+      <c r="M7" s="278"/>
+      <c r="N7" s="278"/>
+      <c r="O7" s="278"/>
+      <c r="P7" s="278"/>
+      <c r="Q7" s="278"/>
     </row>
     <row r="8" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="96">
         <v>3</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="C8" s="88" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="D8" s="88" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
       <c r="E8" s="88" t="s">
-        <v>676</v>
+        <v>669</v>
       </c>
       <c r="F8" s="88" t="s">
-        <v>677</v>
+        <v>670</v>
       </c>
       <c r="G8" s="88" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="H8" s="88" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="I8" s="97" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="14" x14ac:dyDescent="0.3">
@@ -17705,111 +18055,111 @@
       <c r="I14" s="79"/>
     </row>
     <row r="15" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="252" t="s">
-        <v>641</v>
-      </c>
-      <c r="B15" s="253"/>
-      <c r="C15" s="253"/>
-      <c r="D15" s="253"/>
-      <c r="E15" s="253"/>
-      <c r="F15" s="253"/>
-      <c r="G15" s="253"/>
-      <c r="H15" s="253"/>
-      <c r="I15" s="254"/>
+      <c r="A15" s="264" t="s">
+        <v>634</v>
+      </c>
+      <c r="B15" s="265"/>
+      <c r="C15" s="265"/>
+      <c r="D15" s="265"/>
+      <c r="E15" s="265"/>
+      <c r="F15" s="265"/>
+      <c r="G15" s="265"/>
+      <c r="H15" s="265"/>
+      <c r="I15" s="266"/>
     </row>
     <row r="16" spans="1:17" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" s="85" t="s">
+        <v>628</v>
+      </c>
+      <c r="B16" s="86" t="s">
+        <v>631</v>
+      </c>
+      <c r="C16" s="86" t="s">
+        <v>632</v>
+      </c>
+      <c r="D16" s="86" t="s">
+        <v>633</v>
+      </c>
+      <c r="E16" s="279" t="s">
         <v>635</v>
       </c>
-      <c r="B16" s="86" t="s">
-        <v>638</v>
-      </c>
-      <c r="C16" s="86" t="s">
-        <v>639</v>
-      </c>
-      <c r="D16" s="86" t="s">
-        <v>640</v>
-      </c>
-      <c r="E16" s="267" t="s">
-        <v>642</v>
-      </c>
-      <c r="F16" s="260"/>
-      <c r="G16" s="267" t="s">
-        <v>643</v>
-      </c>
-      <c r="H16" s="261"/>
-      <c r="I16" s="262"/>
+      <c r="F16" s="272"/>
+      <c r="G16" s="279" t="s">
+        <v>636</v>
+      </c>
+      <c r="H16" s="273"/>
+      <c r="I16" s="274"/>
     </row>
     <row r="17" spans="1:11" ht="14" x14ac:dyDescent="0.3">
       <c r="A17" s="91">
         <v>1</v>
       </c>
       <c r="B17" s="88" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="C17" s="88" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="D17" s="88" t="s">
-        <v>654</v>
-      </c>
-      <c r="E17" s="268" t="s">
-        <v>652</v>
-      </c>
-      <c r="F17" s="260"/>
-      <c r="G17" s="268" t="s">
-        <v>680</v>
-      </c>
-      <c r="H17" s="261"/>
-      <c r="I17" s="262"/>
+        <v>647</v>
+      </c>
+      <c r="E17" s="280" t="s">
+        <v>645</v>
+      </c>
+      <c r="F17" s="272"/>
+      <c r="G17" s="280" t="s">
+        <v>673</v>
+      </c>
+      <c r="H17" s="273"/>
+      <c r="I17" s="274"/>
     </row>
     <row r="18" spans="1:11" ht="21" x14ac:dyDescent="0.3">
       <c r="A18" s="91">
         <v>2</v>
       </c>
       <c r="B18" s="88" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="C18" s="88" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="D18" s="88" t="s">
-        <v>654</v>
-      </c>
-      <c r="E18" s="268" t="s">
-        <v>652</v>
-      </c>
-      <c r="F18" s="260"/>
-      <c r="G18" s="268" t="s">
-        <v>681</v>
-      </c>
-      <c r="H18" s="261"/>
-      <c r="I18" s="262"/>
+        <v>647</v>
+      </c>
+      <c r="E18" s="280" t="s">
+        <v>645</v>
+      </c>
+      <c r="F18" s="272"/>
+      <c r="G18" s="280" t="s">
+        <v>674</v>
+      </c>
+      <c r="H18" s="273"/>
+      <c r="I18" s="274"/>
     </row>
     <row r="19" spans="1:11" ht="31.5" x14ac:dyDescent="0.35">
       <c r="A19" s="91">
         <v>3</v>
       </c>
       <c r="B19" s="88" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="C19" s="88" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="D19" s="88" t="s">
-        <v>645</v>
-      </c>
-      <c r="E19" s="268" t="s">
-        <v>683</v>
-      </c>
-      <c r="F19" s="260"/>
-      <c r="G19" s="268" t="s">
-        <v>684</v>
-      </c>
-      <c r="H19" s="261"/>
-      <c r="I19" s="262"/>
+        <v>638</v>
+      </c>
+      <c r="E19" s="280" t="s">
+        <v>676</v>
+      </c>
+      <c r="F19" s="272"/>
+      <c r="G19" s="280" t="s">
+        <v>677</v>
+      </c>
+      <c r="H19" s="273"/>
+      <c r="I19" s="274"/>
       <c r="K19" s="84" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.5" x14ac:dyDescent="0.35">
@@ -17819,11 +18169,11 @@
       <c r="B20" s="92"/>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
-      <c r="E20" s="259"/>
-      <c r="F20" s="260"/>
-      <c r="G20" s="259"/>
-      <c r="H20" s="261"/>
-      <c r="I20" s="262"/>
+      <c r="E20" s="271"/>
+      <c r="F20" s="272"/>
+      <c r="G20" s="271"/>
+      <c r="H20" s="273"/>
+      <c r="I20" s="274"/>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="91">
@@ -17832,13 +18182,13 @@
       <c r="B21" s="92"/>
       <c r="C21" s="92"/>
       <c r="D21" s="92"/>
-      <c r="E21" s="259"/>
-      <c r="F21" s="260"/>
-      <c r="G21" s="259"/>
-      <c r="H21" s="261"/>
-      <c r="I21" s="262"/>
+      <c r="E21" s="271"/>
+      <c r="F21" s="272"/>
+      <c r="G21" s="271"/>
+      <c r="H21" s="273"/>
+      <c r="I21" s="274"/>
       <c r="K21" s="84" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -17848,11 +18198,11 @@
       <c r="B22" s="92"/>
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
-      <c r="E22" s="259"/>
-      <c r="F22" s="260"/>
-      <c r="G22" s="259"/>
-      <c r="H22" s="261"/>
-      <c r="I22" s="262"/>
+      <c r="E22" s="271"/>
+      <c r="F22" s="272"/>
+      <c r="G22" s="271"/>
+      <c r="H22" s="273"/>
+      <c r="I22" s="274"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="91">
@@ -17861,11 +18211,11 @@
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
       <c r="D23" s="92"/>
-      <c r="E23" s="259"/>
-      <c r="F23" s="260"/>
-      <c r="G23" s="259"/>
-      <c r="H23" s="261"/>
-      <c r="I23" s="262"/>
+      <c r="E23" s="271"/>
+      <c r="F23" s="272"/>
+      <c r="G23" s="271"/>
+      <c r="H23" s="273"/>
+      <c r="I23" s="274"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="91">
@@ -17874,11 +18224,11 @@
       <c r="B24" s="92"/>
       <c r="C24" s="92"/>
       <c r="D24" s="92"/>
-      <c r="E24" s="259"/>
-      <c r="F24" s="260"/>
-      <c r="G24" s="259"/>
-      <c r="H24" s="261"/>
-      <c r="I24" s="262"/>
+      <c r="E24" s="271"/>
+      <c r="F24" s="272"/>
+      <c r="G24" s="271"/>
+      <c r="H24" s="273"/>
+      <c r="I24" s="274"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="91">
@@ -17887,11 +18237,11 @@
       <c r="B25" s="93"/>
       <c r="C25" s="93"/>
       <c r="D25" s="93"/>
-      <c r="E25" s="263"/>
-      <c r="F25" s="260"/>
-      <c r="G25" s="263"/>
-      <c r="H25" s="261"/>
-      <c r="I25" s="262"/>
+      <c r="E25" s="275"/>
+      <c r="F25" s="272"/>
+      <c r="G25" s="275"/>
+      <c r="H25" s="273"/>
+      <c r="I25" s="274"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="94">
@@ -17900,11 +18250,11 @@
       <c r="B26" s="95"/>
       <c r="C26" s="95"/>
       <c r="D26" s="95"/>
-      <c r="E26" s="264"/>
-      <c r="F26" s="246"/>
-      <c r="G26" s="264"/>
-      <c r="H26" s="248"/>
-      <c r="I26" s="250"/>
+      <c r="E26" s="276"/>
+      <c r="F26" s="258"/>
+      <c r="G26" s="276"/>
+      <c r="H26" s="260"/>
+      <c r="I26" s="262"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -18935,75 +19285,75 @@
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="J1" s="84" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="269" t="s">
-        <v>687</v>
-      </c>
-      <c r="B5" s="261"/>
-      <c r="C5" s="260"/>
+      <c r="A5" s="281" t="s">
+        <v>680</v>
+      </c>
+      <c r="B5" s="273"/>
+      <c r="C5" s="272"/>
     </row>
     <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="101" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="B6" s="101" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="C6" s="101" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="102" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="B7" s="92" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
       <c r="C7" s="103" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="58" x14ac:dyDescent="0.3">
       <c r="A8" s="104" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="B8" s="105" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="106" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="B9" s="107" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="C9" s="103" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="108" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="C10" s="103" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="270"/>
-      <c r="B12" s="266"/>
-      <c r="C12" s="266"/>
+      <c r="A12" s="282"/>
+      <c r="B12" s="278"/>
+      <c r="C12" s="278"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="109"/>
@@ -20037,20 +20387,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="271" t="s">
-        <v>698</v>
-      </c>
-      <c r="C2" s="260"/>
+      <c r="B2" s="283" t="s">
+        <v>691</v>
+      </c>
+      <c r="C2" s="272"/>
       <c r="O2" s="84" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="116" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="C3" s="117" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -20058,10 +20408,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="119" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="D4" s="84" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20069,10 +20419,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="119" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="D5" s="84" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20080,10 +20430,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="119" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="D6" s="84" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20091,10 +20441,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="119" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="D7" s="84" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
     </row>
     <row r="8" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20102,10 +20452,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="119" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="D8" s="84" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
     </row>
     <row r="9" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20113,10 +20463,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="119" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D9" s="84" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
     </row>
     <row r="10" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20124,10 +20474,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="119" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="D10" s="84" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
     </row>
     <row r="11" spans="2:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -20135,10 +20485,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="119" t="s">
-        <v>715</v>
+        <v>708</v>
       </c>
       <c r="D11" s="84" t="s">
-        <v>716</v>
+        <v>709</v>
       </c>
     </row>
     <row r="12" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20146,10 +20496,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="119" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="D12" s="84" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
     </row>
     <row r="13" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20157,10 +20507,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="119" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="D13" s="84" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
     </row>
     <row r="14" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20168,10 +20518,10 @@
         <v>11</v>
       </c>
       <c r="C14" s="119" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
       <c r="D14" s="84" t="s">
-        <v>722</v>
+        <v>715</v>
       </c>
     </row>
     <row r="15" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20179,10 +20529,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="119" t="s">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="D15" s="84" t="s">
-        <v>724</v>
+        <v>717</v>
       </c>
     </row>
     <row r="16" spans="2:15" ht="14.5" x14ac:dyDescent="0.35">
@@ -20190,10 +20540,10 @@
         <v>13</v>
       </c>
       <c r="C16" s="119" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>726</v>
+        <v>719</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="14.5" x14ac:dyDescent="0.35">
@@ -20201,10 +20551,10 @@
         <v>14</v>
       </c>
       <c r="C17" s="119" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="14.5" x14ac:dyDescent="0.35">
@@ -20251,7 +20601,7 @@
     <row r="30" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C31" s="84" t="s">
-        <v>729</v>
+        <v>722</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -21249,73 +21599,73 @@
   <sheetData>
     <row r="2" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="J2" s="84" t="s">
-        <v>730</v>
+        <v>723</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="271" t="s">
-        <v>731</v>
-      </c>
-      <c r="B3" s="261"/>
-      <c r="C3" s="260"/>
+      <c r="A3" s="283" t="s">
+        <v>724</v>
+      </c>
+      <c r="B3" s="273"/>
+      <c r="C3" s="272"/>
     </row>
     <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="101" t="s">
-        <v>635</v>
-      </c>
-      <c r="B4" s="269" t="s">
-        <v>732</v>
-      </c>
-      <c r="C4" s="260"/>
+        <v>628</v>
+      </c>
+      <c r="B4" s="281" t="s">
+        <v>725</v>
+      </c>
+      <c r="C4" s="272"/>
     </row>
     <row r="5" spans="1:10" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="120" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="272" t="s">
-        <v>733</v>
-      </c>
-      <c r="C5" s="260"/>
+      <c r="B5" s="284" t="s">
+        <v>726</v>
+      </c>
+      <c r="C5" s="272"/>
     </row>
     <row r="6" spans="1:10" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="120" t="s">
         <v>131</v>
       </c>
-      <c r="B6" s="272" t="s">
-        <v>734</v>
-      </c>
-      <c r="C6" s="260"/>
+      <c r="B6" s="284" t="s">
+        <v>727</v>
+      </c>
+      <c r="C6" s="272"/>
     </row>
     <row r="7" spans="1:10" ht="67.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="120" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="272" t="s">
-        <v>735</v>
-      </c>
-      <c r="C7" s="260"/>
+      <c r="B7" s="284" t="s">
+        <v>728</v>
+      </c>
+      <c r="C7" s="272"/>
     </row>
     <row r="8" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="120" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="272" t="s">
-        <v>736</v>
-      </c>
-      <c r="C8" s="260"/>
+      <c r="B8" s="284" t="s">
+        <v>729</v>
+      </c>
+      <c r="C8" s="272"/>
     </row>
     <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B13" s="271" t="s">
-        <v>698</v>
-      </c>
-      <c r="C13" s="260"/>
+      <c r="B13" s="283" t="s">
+        <v>691</v>
+      </c>
+      <c r="C13" s="272"/>
     </row>
     <row r="14" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B14" s="116" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
       <c r="C14" s="117" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
@@ -21323,10 +21673,10 @@
         <v>1</v>
       </c>
       <c r="C15" s="119" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
       <c r="D15" s="84" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
@@ -21334,10 +21684,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="119" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="D16" s="84" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="14.5" x14ac:dyDescent="0.35">
@@ -21345,10 +21695,10 @@
         <v>3</v>
       </c>
       <c r="C17" s="119" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
       <c r="D17" s="84" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="14.5" x14ac:dyDescent="0.35">
@@ -21356,10 +21706,10 @@
         <v>4</v>
       </c>
       <c r="C18" s="119" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
       <c r="D18" s="84" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="14.5" x14ac:dyDescent="0.35">
@@ -21367,10 +21717,10 @@
         <v>5</v>
       </c>
       <c r="C19" s="119" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
       <c r="D19" s="84" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="14.5" x14ac:dyDescent="0.35">
@@ -21378,10 +21728,10 @@
         <v>6</v>
       </c>
       <c r="C20" s="119" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
       <c r="D20" s="84" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -21389,10 +21739,10 @@
         <v>7</v>
       </c>
       <c r="C21" s="119" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
       <c r="D21" s="84" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -21400,10 +21750,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="119" t="s">
-        <v>715</v>
+        <v>708</v>
       </c>
       <c r="D22" s="84" t="s">
-        <v>716</v>
+        <v>709</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -21411,10 +21761,10 @@
         <v>9</v>
       </c>
       <c r="C23" s="119" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="D23" s="84" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -21422,10 +21772,10 @@
         <v>10</v>
       </c>
       <c r="C24" s="119" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="D24" s="84" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
     </row>
     <row r="25" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -21433,10 +21783,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="119" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
       <c r="D25" s="84" t="s">
-        <v>722</v>
+        <v>715</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -21444,10 +21794,10 @@
         <v>12</v>
       </c>
       <c r="C26" s="119" t="s">
-        <v>723</v>
+        <v>716</v>
       </c>
       <c r="D26" s="84" t="s">
-        <v>724</v>
+        <v>717</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -21455,10 +21805,10 @@
         <v>13</v>
       </c>
       <c r="C27" s="119" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="D27" s="84" t="s">
-        <v>726</v>
+        <v>719</v>
       </c>
     </row>
     <row r="28" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -21466,10 +21816,10 @@
         <v>14</v>
       </c>
       <c r="C28" s="119" t="s">
-        <v>727</v>
+        <v>720</v>
       </c>
       <c r="D28" s="84" t="s">
-        <v>728</v>
+        <v>721</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -22506,112 +22856,112 @@
       <c r="D1" s="36"/>
     </row>
     <row r="2" spans="2:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="273" t="s">
-        <v>737</v>
-      </c>
-      <c r="C2" s="243"/>
-      <c r="D2" s="244"/>
+      <c r="B2" s="285" t="s">
+        <v>730</v>
+      </c>
+      <c r="C2" s="255"/>
+      <c r="D2" s="256"/>
       <c r="J2" s="84" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="121" t="s">
-        <v>738</v>
+        <v>731</v>
       </c>
       <c r="C3" s="117" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="D3" s="122" t="s">
-        <v>739</v>
+        <v>732</v>
       </c>
     </row>
     <row r="4" spans="2:10" ht="87" x14ac:dyDescent="0.3">
       <c r="B4" s="123" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="C4" s="103" t="s">
-        <v>740</v>
+        <v>733</v>
       </c>
       <c r="D4" s="124" t="s">
-        <v>741</v>
+        <v>734</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5" s="123" t="s">
-        <v>742</v>
+        <v>735</v>
       </c>
       <c r="C5" s="103" t="s">
-        <v>743</v>
+        <v>736</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>744</v>
+        <v>737</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="123" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="C6" s="103" t="s">
-        <v>745</v>
+        <v>738</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>746</v>
+        <v>739</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B7" s="123" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="C7" s="107" t="s">
-        <v>747</v>
+        <v>740</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>748</v>
+        <v>741</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B8" s="123" t="s">
-        <v>749</v>
+        <v>742</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>750</v>
+        <v>743</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>751</v>
+        <v>744</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="123" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="C9" s="103" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="D9" s="125" t="s">
-        <v>753</v>
+        <v>746</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B10" s="123" t="s">
-        <v>754</v>
+        <v>747</v>
       </c>
       <c r="C10" s="107" t="s">
-        <v>755</v>
+        <v>748</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>756</v>
+        <v>749</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="126" t="s">
-        <v>757</v>
+        <v>750</v>
       </c>
       <c r="C11" s="127" t="s">
-        <v>758</v>
+        <v>751</v>
       </c>
       <c r="D11" s="128" t="s">
-        <v>759</v>
+        <v>752</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="14.5" x14ac:dyDescent="0.35">
@@ -25606,24 +25956,24 @@
   <sheetData>
     <row r="2" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B2" s="84" t="s">
-        <v>760</v>
+        <v>753</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B3" s="84" t="s">
-        <v>761</v>
+        <v>754</v>
       </c>
       <c r="C3" s="129" t="s">
-        <v>762</v>
+        <v>755</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="6.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B5" s="84" t="s">
-        <v>763</v>
+        <v>756</v>
       </c>
       <c r="C5" s="129" t="s">
-        <v>764</v>
+        <v>757</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -26640,20 +26990,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="49.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="239" t="s">
+      <c r="A1" s="251" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="241"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="252"/>
+      <c r="H1" s="253"/>
     </row>
     <row r="2" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="B2" s="130"/>
       <c r="C2" s="3"/>
@@ -26715,7 +27065,7 @@
         <v>15</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -26770,7 +27120,7 @@
         <v>25</v>
       </c>
       <c r="L6" s="37" t="s">
-        <v>767</v>
+        <v>760</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
@@ -26825,7 +27175,7 @@
         <v>38</v>
       </c>
       <c r="K8" s="33" t="s">
-        <v>768</v>
+        <v>761</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
@@ -27189,7 +27539,7 @@
         <v>116</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>769</v>
+        <v>762</v>
       </c>
       <c r="C22" s="51">
         <v>9</v>
@@ -27215,7 +27565,7 @@
         <v>123</v>
       </c>
       <c r="B23" s="28" t="s">
-        <v>769</v>
+        <v>762</v>
       </c>
       <c r="C23" s="52">
         <v>9</v>
@@ -27259,7 +27609,7 @@
         <v>134</v>
       </c>
       <c r="H24" s="25" t="s">
-        <v>770</v>
+        <v>763</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -27270,7 +27620,7 @@
         <v>137</v>
       </c>
       <c r="C25" s="52" t="s">
-        <v>771</v>
+        <v>764</v>
       </c>
       <c r="D25" s="27" t="s">
         <v>34</v>
@@ -27285,7 +27635,7 @@
         <v>140</v>
       </c>
       <c r="H25" s="29" t="s">
-        <v>772</v>
+        <v>765</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -27296,7 +27646,7 @@
         <v>143</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>771</v>
+        <v>764</v>
       </c>
       <c r="D26" s="23" t="s">
         <v>34</v>
@@ -27556,7 +27906,7 @@
         <v>201</v>
       </c>
       <c r="B36" s="24" t="s">
-        <v>773</v>
+        <v>766</v>
       </c>
       <c r="C36" s="51">
         <v>9</v>
@@ -27585,7 +27935,7 @@
         <v>208</v>
       </c>
       <c r="C37" s="52" t="s">
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="D37" s="39" t="s">
         <v>11</v>
@@ -27611,7 +27961,7 @@
         <v>215</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>11</v>
@@ -27736,7 +28086,7 @@
         <v>242</v>
       </c>
       <c r="J42" s="37" t="s">
-        <v>775</v>
+        <v>768</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -27791,7 +28141,7 @@
         <v>254</v>
       </c>
       <c r="J44" s="37" t="s">
-        <v>776</v>
+        <v>769</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -28183,7 +28533,7 @@
         <v>332</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>777</v>
+        <v>770</v>
       </c>
       <c r="C60" s="51">
         <v>1</v>
@@ -28209,7 +28559,7 @@
         <v>338</v>
       </c>
       <c r="B61" s="28" t="s">
-        <v>778</v>
+        <v>771</v>
       </c>
       <c r="C61" s="52">
         <v>1</v>
@@ -28235,7 +28585,7 @@
         <v>345</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>778</v>
+        <v>771</v>
       </c>
       <c r="C62" s="132">
         <v>1</v>
@@ -28264,7 +28614,7 @@
         <v>352</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>779</v>
+        <v>772</v>
       </c>
       <c r="C63" s="52">
         <v>1</v>
@@ -28290,7 +28640,7 @@
         <v>358</v>
       </c>
       <c r="B64" s="33" t="s">
-        <v>780</v>
+        <v>773</v>
       </c>
       <c r="C64" s="51">
         <v>1</v>
@@ -28493,7 +28843,7 @@
         <v>407</v>
       </c>
       <c r="J71" s="37" t="s">
-        <v>781</v>
+        <v>774</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -28813,7 +29163,7 @@
         <v>475</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>782</v>
+        <v>775</v>
       </c>
       <c r="C84" s="31">
         <v>5</v>
@@ -28839,7 +29189,7 @@
         <v>481</v>
       </c>
       <c r="B85" s="28" t="s">
-        <v>783</v>
+        <v>776</v>
       </c>
       <c r="C85" s="63">
         <v>8</v>
@@ -28865,7 +29215,7 @@
         <v>488</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>784</v>
+        <v>777</v>
       </c>
       <c r="C86" s="31">
         <v>8</v>
@@ -28917,7 +29267,7 @@
         <v>502</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="C88" s="31">
         <v>7</v>
@@ -28969,7 +29319,7 @@
         <v>513</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="C90" s="31">
         <v>7</v>
@@ -29021,7 +29371,7 @@
         <v>525</v>
       </c>
       <c r="B92" s="24" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="C92" s="31">
         <v>7</v>
@@ -29039,7 +29389,7 @@
         <v>529</v>
       </c>
       <c r="H92" s="25" t="s">
-        <v>786</v>
+        <v>779</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>